<commit_message>
nmv 10 04 2022
</commit_message>
<xml_diff>
--- a/TS Jatai Ghanam Project/Stas table for TS 2.1 TO 2.6.xlsx
+++ b/TS Jatai Ghanam Project/Stas table for TS 2.1 TO 2.6.xlsx
@@ -13,7 +13,8 @@
   </bookViews>
   <sheets>
     <sheet name="TS 2.1" sheetId="8" r:id="rId1"/>
-    <sheet name="total 2.1 to 2.6" sheetId="7" r:id="rId2"/>
+    <sheet name="TS 2.2" sheetId="9" r:id="rId2"/>
+    <sheet name="total 2.1 to 2.6" sheetId="7" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="180">
   <si>
     <t>Panchaati Ref</t>
   </si>
@@ -1455,13 +1456,229 @@
   </si>
   <si>
     <t xml:space="preserve">No. of Padams as per Pada PaaTam </t>
+  </si>
+  <si>
+    <t>2.2.1.1 :</t>
+  </si>
+  <si>
+    <t>2.2.1.2 :</t>
+  </si>
+  <si>
+    <t>2.2.1.3 :</t>
+  </si>
+  <si>
+    <t>2.2.1.4 :</t>
+  </si>
+  <si>
+    <t>2.2.1.5 :</t>
+  </si>
+  <si>
+    <t>2.2.2.1 :</t>
+  </si>
+  <si>
+    <t>2.2.2.2 :</t>
+  </si>
+  <si>
+    <t>2.2.2.3 :</t>
+  </si>
+  <si>
+    <t>2.2.2.4 :</t>
+  </si>
+  <si>
+    <t>2.2.2.5 :</t>
+  </si>
+  <si>
+    <t>2.2.3.1 :</t>
+  </si>
+  <si>
+    <t>2.2.3.2 :</t>
+  </si>
+  <si>
+    <t>2.2.3.3 :</t>
+  </si>
+  <si>
+    <t>2.2.3.4 :</t>
+  </si>
+  <si>
+    <t>2.2.4.1 :</t>
+  </si>
+  <si>
+    <t>2.2.4.2 :</t>
+  </si>
+  <si>
+    <t>2.2.4.3 :</t>
+  </si>
+  <si>
+    <t>2.2.4.4 :</t>
+  </si>
+  <si>
+    <t>2.2.4.5 :</t>
+  </si>
+  <si>
+    <t>2.2.4.6 :</t>
+  </si>
+  <si>
+    <t>2.2.4.7 :</t>
+  </si>
+  <si>
+    <t>2.2.4.8 :</t>
+  </si>
+  <si>
+    <t>2.2.5.1 :</t>
+  </si>
+  <si>
+    <t>2.2.5.2 :</t>
+  </si>
+  <si>
+    <t>2.2.5.3 :</t>
+  </si>
+  <si>
+    <t>2.2.5.4 :</t>
+  </si>
+  <si>
+    <t>2.2.5.5 :</t>
+  </si>
+  <si>
+    <t>2.2.5.6 :</t>
+  </si>
+  <si>
+    <t>2.2.5.7 :</t>
+  </si>
+  <si>
+    <t>2.2.6.1 :</t>
+  </si>
+  <si>
+    <t>2.2.6.2 :</t>
+  </si>
+  <si>
+    <t>2.2.6.3 :</t>
+  </si>
+  <si>
+    <t>2.2.6.4 :</t>
+  </si>
+  <si>
+    <t>2.2.6.5 :</t>
+  </si>
+  <si>
+    <t>2.2.7.1 :</t>
+  </si>
+  <si>
+    <t>2.2.7.2 :</t>
+  </si>
+  <si>
+    <t>2.2.7.3 :</t>
+  </si>
+  <si>
+    <t>2.2.7.4 :</t>
+  </si>
+  <si>
+    <t>2.2.7.5 :</t>
+  </si>
+  <si>
+    <t>2.2.8.1 :</t>
+  </si>
+  <si>
+    <t>2.2.8.2 :</t>
+  </si>
+  <si>
+    <t>2.2.8.3 :</t>
+  </si>
+  <si>
+    <t>2.2.8.4 :</t>
+  </si>
+  <si>
+    <t>2.2.8.5 :</t>
+  </si>
+  <si>
+    <t>2.2.8.6 :</t>
+  </si>
+  <si>
+    <t>2.2.9.1 :</t>
+  </si>
+  <si>
+    <t>2.2.9.2 :</t>
+  </si>
+  <si>
+    <t>2.2.9.3 :</t>
+  </si>
+  <si>
+    <t>2.2.9.4 :</t>
+  </si>
+  <si>
+    <t>2.2.9.5 :</t>
+  </si>
+  <si>
+    <t>2.2.9.6 :</t>
+  </si>
+  <si>
+    <t>2.2.9.7 :</t>
+  </si>
+  <si>
+    <t>2.2.10.1 :</t>
+  </si>
+  <si>
+    <t>2.2.10.2 :</t>
+  </si>
+  <si>
+    <t>2.2.10.3 :</t>
+  </si>
+  <si>
+    <t>2.2.10.4 :</t>
+  </si>
+  <si>
+    <t>2.2.10.5 :</t>
+  </si>
+  <si>
+    <t>2.2.11.1 :</t>
+  </si>
+  <si>
+    <t>2.2.11.2 :</t>
+  </si>
+  <si>
+    <t>2.2.11.3 :</t>
+  </si>
+  <si>
+    <t>2.2.11.4 :</t>
+  </si>
+  <si>
+    <t>2.2.11.5 :</t>
+  </si>
+  <si>
+    <t>2.2.11.6 :</t>
+  </si>
+  <si>
+    <t>2.2.12.1 :</t>
+  </si>
+  <si>
+    <t>2.2.12.2 :</t>
+  </si>
+  <si>
+    <t>2.2.12.3 :</t>
+  </si>
+  <si>
+    <t>2.2.12.4 :</t>
+  </si>
+  <si>
+    <t>2.2.12.5 :</t>
+  </si>
+  <si>
+    <t>2.2.12.6 :</t>
+  </si>
+  <si>
+    <t>2.2.12.7 :</t>
+  </si>
+  <si>
+    <t>2.2.12.8 :</t>
+  </si>
+  <si>
+    <t>71</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1525,6 +1742,25 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="6">
@@ -1610,7 +1846,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
@@ -1675,6 +1911,19 @@
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="46" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1959,7 +2208,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A65" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A67" sqref="A67:L67"/>
+      <selection pane="bottomLeft" activeCell="E68" sqref="E68:J77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4701,9 +4950,2926 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:L83"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A68" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" sqref="A1:L73"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.85546875" customWidth="1"/>
+    <col min="3" max="3" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="4.42578125" customWidth="1"/>
+    <col min="5" max="5" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="6.5703125" customWidth="1"/>
+    <col min="8" max="8" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="4.140625" customWidth="1"/>
+    <col min="11" max="11" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" ht="89.25" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A2" s="25" t="s">
+        <v>108</v>
+      </c>
+      <c r="B2" s="25">
+        <v>13</v>
+      </c>
+      <c r="C2" s="25">
+        <v>0</v>
+      </c>
+      <c r="D2" s="25">
+        <v>4</v>
+      </c>
+      <c r="E2" s="25">
+        <v>0</v>
+      </c>
+      <c r="F2" s="25">
+        <v>0</v>
+      </c>
+      <c r="G2" s="25">
+        <v>6</v>
+      </c>
+      <c r="H2" s="25">
+        <v>0</v>
+      </c>
+      <c r="I2" s="25">
+        <v>0</v>
+      </c>
+      <c r="J2" s="25">
+        <v>33</v>
+      </c>
+      <c r="K2" s="25">
+        <v>50</v>
+      </c>
+      <c r="L2" s="25">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A3" s="25" t="s">
+        <v>109</v>
+      </c>
+      <c r="B3" s="25">
+        <v>11</v>
+      </c>
+      <c r="C3" s="25">
+        <v>0</v>
+      </c>
+      <c r="D3" s="25">
+        <v>1</v>
+      </c>
+      <c r="E3" s="25">
+        <v>0</v>
+      </c>
+      <c r="F3" s="25">
+        <v>0</v>
+      </c>
+      <c r="G3" s="25">
+        <v>7</v>
+      </c>
+      <c r="H3" s="25">
+        <v>0</v>
+      </c>
+      <c r="I3" s="25">
+        <v>0</v>
+      </c>
+      <c r="J3" s="25">
+        <v>38</v>
+      </c>
+      <c r="K3" s="25">
+        <v>50</v>
+      </c>
+      <c r="L3" s="25">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A4" s="25" t="s">
+        <v>110</v>
+      </c>
+      <c r="B4" s="25">
+        <v>9</v>
+      </c>
+      <c r="C4" s="25">
+        <v>0</v>
+      </c>
+      <c r="D4" s="25">
+        <v>2</v>
+      </c>
+      <c r="E4" s="25">
+        <v>0</v>
+      </c>
+      <c r="F4" s="25">
+        <v>0</v>
+      </c>
+      <c r="G4" s="25">
+        <v>5</v>
+      </c>
+      <c r="H4" s="25">
+        <v>0</v>
+      </c>
+      <c r="I4" s="25">
+        <v>0</v>
+      </c>
+      <c r="J4" s="25">
+        <v>39</v>
+      </c>
+      <c r="K4" s="25">
+        <v>50</v>
+      </c>
+      <c r="L4" s="25">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A5" s="25" t="s">
+        <v>111</v>
+      </c>
+      <c r="B5" s="25">
+        <v>4</v>
+      </c>
+      <c r="C5" s="25">
+        <v>0</v>
+      </c>
+      <c r="D5" s="25">
+        <v>1</v>
+      </c>
+      <c r="E5" s="25">
+        <v>0</v>
+      </c>
+      <c r="F5" s="25">
+        <v>0</v>
+      </c>
+      <c r="G5" s="25">
+        <v>6</v>
+      </c>
+      <c r="H5" s="25">
+        <v>0</v>
+      </c>
+      <c r="I5" s="25">
+        <v>0</v>
+      </c>
+      <c r="J5" s="25">
+        <v>45</v>
+      </c>
+      <c r="K5" s="25">
+        <v>50</v>
+      </c>
+      <c r="L5" s="25">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A6" s="25" t="s">
+        <v>112</v>
+      </c>
+      <c r="B6" s="25">
+        <v>6</v>
+      </c>
+      <c r="C6" s="25">
+        <v>0</v>
+      </c>
+      <c r="D6" s="25">
+        <v>0</v>
+      </c>
+      <c r="E6" s="25">
+        <v>0</v>
+      </c>
+      <c r="F6" s="25">
+        <v>1</v>
+      </c>
+      <c r="G6" s="25">
+        <v>4</v>
+      </c>
+      <c r="H6" s="25">
+        <v>0</v>
+      </c>
+      <c r="I6" s="25">
+        <v>0</v>
+      </c>
+      <c r="J6" s="25">
+        <v>32</v>
+      </c>
+      <c r="K6" s="25">
+        <v>39</v>
+      </c>
+      <c r="L6" s="25">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A7" s="25" t="s">
+        <v>113</v>
+      </c>
+      <c r="B7" s="25">
+        <v>14</v>
+      </c>
+      <c r="C7" s="25">
+        <v>0</v>
+      </c>
+      <c r="D7" s="25">
+        <v>0</v>
+      </c>
+      <c r="E7" s="25">
+        <v>0</v>
+      </c>
+      <c r="F7" s="25">
+        <v>0</v>
+      </c>
+      <c r="G7" s="25">
+        <v>4</v>
+      </c>
+      <c r="H7" s="25">
+        <v>0</v>
+      </c>
+      <c r="I7" s="25">
+        <v>0</v>
+      </c>
+      <c r="J7" s="25">
+        <v>36</v>
+      </c>
+      <c r="K7" s="25">
+        <v>50</v>
+      </c>
+      <c r="L7" s="25">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A8" s="25" t="s">
+        <v>114</v>
+      </c>
+      <c r="B8" s="25">
+        <v>9</v>
+      </c>
+      <c r="C8" s="25">
+        <v>0</v>
+      </c>
+      <c r="D8" s="25">
+        <v>0</v>
+      </c>
+      <c r="E8" s="25">
+        <v>0</v>
+      </c>
+      <c r="F8" s="25">
+        <v>0</v>
+      </c>
+      <c r="G8" s="25">
+        <v>7</v>
+      </c>
+      <c r="H8" s="25">
+        <v>0</v>
+      </c>
+      <c r="I8" s="25">
+        <v>0</v>
+      </c>
+      <c r="J8" s="25">
+        <v>41</v>
+      </c>
+      <c r="K8" s="25">
+        <v>50</v>
+      </c>
+      <c r="L8" s="25">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A9" s="25" t="s">
+        <v>115</v>
+      </c>
+      <c r="B9" s="25">
+        <v>10</v>
+      </c>
+      <c r="C9" s="25">
+        <v>0</v>
+      </c>
+      <c r="D9" s="25">
+        <v>2</v>
+      </c>
+      <c r="E9" s="25">
+        <v>0</v>
+      </c>
+      <c r="F9" s="25">
+        <v>0</v>
+      </c>
+      <c r="G9" s="25">
+        <v>4</v>
+      </c>
+      <c r="H9" s="25">
+        <v>0</v>
+      </c>
+      <c r="I9" s="25">
+        <v>0</v>
+      </c>
+      <c r="J9" s="25">
+        <v>38</v>
+      </c>
+      <c r="K9" s="25">
+        <v>50</v>
+      </c>
+      <c r="L9" s="25">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A10" s="25" t="s">
+        <v>116</v>
+      </c>
+      <c r="B10" s="25">
+        <v>11</v>
+      </c>
+      <c r="C10" s="25">
+        <v>0</v>
+      </c>
+      <c r="D10" s="25">
+        <v>0</v>
+      </c>
+      <c r="E10" s="25">
+        <v>0</v>
+      </c>
+      <c r="F10" s="25">
+        <v>0</v>
+      </c>
+      <c r="G10" s="25">
+        <v>3</v>
+      </c>
+      <c r="H10" s="25">
+        <v>0</v>
+      </c>
+      <c r="I10" s="25">
+        <v>0</v>
+      </c>
+      <c r="J10" s="25">
+        <v>39</v>
+      </c>
+      <c r="K10" s="25">
+        <v>50</v>
+      </c>
+      <c r="L10" s="25">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A11" s="25" t="s">
+        <v>117</v>
+      </c>
+      <c r="B11" s="25">
+        <v>10</v>
+      </c>
+      <c r="C11" s="25">
+        <v>0</v>
+      </c>
+      <c r="D11" s="25">
+        <v>0</v>
+      </c>
+      <c r="E11" s="25">
+        <v>0</v>
+      </c>
+      <c r="F11" s="25">
+        <v>1</v>
+      </c>
+      <c r="G11" s="25">
+        <v>5</v>
+      </c>
+      <c r="H11" s="25">
+        <v>0</v>
+      </c>
+      <c r="I11" s="25">
+        <v>0</v>
+      </c>
+      <c r="J11" s="25">
+        <v>43</v>
+      </c>
+      <c r="K11" s="25">
+        <v>54</v>
+      </c>
+      <c r="L11" s="25">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A12" s="25" t="s">
+        <v>118</v>
+      </c>
+      <c r="B12" s="25">
+        <v>6</v>
+      </c>
+      <c r="C12" s="25">
+        <v>0</v>
+      </c>
+      <c r="D12" s="25">
+        <v>0</v>
+      </c>
+      <c r="E12" s="25">
+        <v>0</v>
+      </c>
+      <c r="F12" s="25">
+        <v>0</v>
+      </c>
+      <c r="G12" s="25">
+        <v>6</v>
+      </c>
+      <c r="H12" s="25">
+        <v>0</v>
+      </c>
+      <c r="I12" s="25">
+        <v>0</v>
+      </c>
+      <c r="J12" s="25">
+        <v>44</v>
+      </c>
+      <c r="K12" s="25">
+        <v>50</v>
+      </c>
+      <c r="L12" s="25">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A13" s="25" t="s">
+        <v>119</v>
+      </c>
+      <c r="B13" s="25">
+        <v>6</v>
+      </c>
+      <c r="C13" s="25">
+        <v>0</v>
+      </c>
+      <c r="D13" s="25">
+        <v>0</v>
+      </c>
+      <c r="E13" s="25">
+        <v>0</v>
+      </c>
+      <c r="F13" s="25">
+        <v>0</v>
+      </c>
+      <c r="G13" s="25">
+        <v>5</v>
+      </c>
+      <c r="H13" s="25">
+        <v>0</v>
+      </c>
+      <c r="I13" s="25">
+        <v>0</v>
+      </c>
+      <c r="J13" s="25">
+        <v>44</v>
+      </c>
+      <c r="K13" s="25">
+        <v>50</v>
+      </c>
+      <c r="L13" s="25">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A14" s="25" t="s">
+        <v>120</v>
+      </c>
+      <c r="B14" s="25">
+        <v>8</v>
+      </c>
+      <c r="C14" s="25">
+        <v>0</v>
+      </c>
+      <c r="D14" s="25">
+        <v>0</v>
+      </c>
+      <c r="E14" s="25">
+        <v>0</v>
+      </c>
+      <c r="F14" s="25">
+        <v>0</v>
+      </c>
+      <c r="G14" s="25">
+        <v>4</v>
+      </c>
+      <c r="H14" s="25">
+        <v>0</v>
+      </c>
+      <c r="I14" s="25">
+        <v>0</v>
+      </c>
+      <c r="J14" s="25">
+        <v>42</v>
+      </c>
+      <c r="K14" s="25">
+        <v>50</v>
+      </c>
+      <c r="L14" s="25">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A15" s="25" t="s">
+        <v>121</v>
+      </c>
+      <c r="B15" s="25">
+        <v>5</v>
+      </c>
+      <c r="C15" s="25">
+        <v>0</v>
+      </c>
+      <c r="D15" s="25">
+        <v>0</v>
+      </c>
+      <c r="E15" s="25">
+        <v>0</v>
+      </c>
+      <c r="F15" s="25">
+        <v>1</v>
+      </c>
+      <c r="G15" s="25">
+        <v>4</v>
+      </c>
+      <c r="H15" s="25">
+        <v>0</v>
+      </c>
+      <c r="I15" s="25">
+        <v>0</v>
+      </c>
+      <c r="J15" s="25">
+        <v>32</v>
+      </c>
+      <c r="K15" s="25">
+        <v>38</v>
+      </c>
+      <c r="L15" s="25">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A16" s="25" t="s">
+        <v>122</v>
+      </c>
+      <c r="B16" s="25">
+        <v>14</v>
+      </c>
+      <c r="C16" s="25">
+        <v>0</v>
+      </c>
+      <c r="D16" s="25">
+        <v>0</v>
+      </c>
+      <c r="E16" s="25">
+        <v>0</v>
+      </c>
+      <c r="F16" s="25">
+        <v>0</v>
+      </c>
+      <c r="G16" s="25">
+        <v>4</v>
+      </c>
+      <c r="H16" s="25">
+        <v>0</v>
+      </c>
+      <c r="I16" s="25">
+        <v>0</v>
+      </c>
+      <c r="J16" s="25">
+        <v>36</v>
+      </c>
+      <c r="K16" s="25">
+        <v>50</v>
+      </c>
+      <c r="L16" s="25">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A17" s="25" t="s">
+        <v>123</v>
+      </c>
+      <c r="B17" s="25">
+        <v>11</v>
+      </c>
+      <c r="C17" s="25">
+        <v>0</v>
+      </c>
+      <c r="D17" s="25">
+        <v>0</v>
+      </c>
+      <c r="E17" s="25">
+        <v>0</v>
+      </c>
+      <c r="F17" s="25">
+        <v>0</v>
+      </c>
+      <c r="G17" s="25">
+        <v>3</v>
+      </c>
+      <c r="H17" s="25">
+        <v>0</v>
+      </c>
+      <c r="I17" s="25">
+        <v>0</v>
+      </c>
+      <c r="J17" s="25">
+        <v>39</v>
+      </c>
+      <c r="K17" s="25">
+        <v>50</v>
+      </c>
+      <c r="L17" s="25">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A18" s="25" t="s">
+        <v>124</v>
+      </c>
+      <c r="B18" s="25">
+        <v>4</v>
+      </c>
+      <c r="C18" s="25">
+        <v>0</v>
+      </c>
+      <c r="D18" s="25">
+        <v>0</v>
+      </c>
+      <c r="E18" s="25">
+        <v>0</v>
+      </c>
+      <c r="F18" s="25">
+        <v>0</v>
+      </c>
+      <c r="G18" s="25">
+        <v>1</v>
+      </c>
+      <c r="H18" s="25">
+        <v>0</v>
+      </c>
+      <c r="I18" s="25">
+        <v>0</v>
+      </c>
+      <c r="J18" s="25">
+        <v>46</v>
+      </c>
+      <c r="K18" s="25">
+        <v>50</v>
+      </c>
+      <c r="L18" s="25">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A19" s="25" t="s">
+        <v>125</v>
+      </c>
+      <c r="B19" s="25">
+        <v>12</v>
+      </c>
+      <c r="C19" s="25">
+        <v>0</v>
+      </c>
+      <c r="D19" s="25">
+        <v>0</v>
+      </c>
+      <c r="E19" s="25">
+        <v>0</v>
+      </c>
+      <c r="F19" s="25">
+        <v>0</v>
+      </c>
+      <c r="G19" s="25">
+        <v>5</v>
+      </c>
+      <c r="H19" s="25">
+        <v>0</v>
+      </c>
+      <c r="I19" s="25">
+        <v>0</v>
+      </c>
+      <c r="J19" s="25">
+        <v>38</v>
+      </c>
+      <c r="K19" s="25">
+        <v>50</v>
+      </c>
+      <c r="L19" s="25">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A20" s="25" t="s">
+        <v>126</v>
+      </c>
+      <c r="B20" s="25">
+        <v>14</v>
+      </c>
+      <c r="C20" s="25">
+        <v>0</v>
+      </c>
+      <c r="D20" s="25">
+        <v>0</v>
+      </c>
+      <c r="E20" s="25">
+        <v>0</v>
+      </c>
+      <c r="F20" s="25">
+        <v>0</v>
+      </c>
+      <c r="G20" s="25">
+        <v>4</v>
+      </c>
+      <c r="H20" s="25">
+        <v>0</v>
+      </c>
+      <c r="I20" s="25">
+        <v>0</v>
+      </c>
+      <c r="J20" s="25">
+        <v>36</v>
+      </c>
+      <c r="K20" s="25">
+        <v>50</v>
+      </c>
+      <c r="L20" s="25">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A21" s="25" t="s">
+        <v>127</v>
+      </c>
+      <c r="B21" s="25">
+        <v>12</v>
+      </c>
+      <c r="C21" s="25">
+        <v>0</v>
+      </c>
+      <c r="D21" s="25">
+        <v>1</v>
+      </c>
+      <c r="E21" s="25">
+        <v>0</v>
+      </c>
+      <c r="F21" s="25">
+        <v>0</v>
+      </c>
+      <c r="G21" s="25">
+        <v>2</v>
+      </c>
+      <c r="H21" s="25">
+        <v>0</v>
+      </c>
+      <c r="I21" s="25">
+        <v>0</v>
+      </c>
+      <c r="J21" s="25">
+        <v>37</v>
+      </c>
+      <c r="K21" s="25">
+        <v>50</v>
+      </c>
+      <c r="L21" s="25">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A22" s="25" t="s">
+        <v>128</v>
+      </c>
+      <c r="B22" s="25">
+        <v>12</v>
+      </c>
+      <c r="C22" s="25">
+        <v>0</v>
+      </c>
+      <c r="D22" s="25">
+        <v>0</v>
+      </c>
+      <c r="E22" s="25">
+        <v>0</v>
+      </c>
+      <c r="F22" s="25">
+        <v>0</v>
+      </c>
+      <c r="G22" s="25">
+        <v>5</v>
+      </c>
+      <c r="H22" s="25">
+        <v>0</v>
+      </c>
+      <c r="I22" s="25">
+        <v>0</v>
+      </c>
+      <c r="J22" s="25">
+        <v>38</v>
+      </c>
+      <c r="K22" s="25">
+        <v>50</v>
+      </c>
+      <c r="L22" s="25">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A23" s="25" t="s">
+        <v>129</v>
+      </c>
+      <c r="B23" s="25">
+        <v>8</v>
+      </c>
+      <c r="C23" s="25">
+        <v>1</v>
+      </c>
+      <c r="D23" s="25">
+        <v>0</v>
+      </c>
+      <c r="E23" s="25">
+        <v>0</v>
+      </c>
+      <c r="F23" s="25">
+        <v>2</v>
+      </c>
+      <c r="G23" s="25">
+        <v>3</v>
+      </c>
+      <c r="H23" s="25">
+        <v>0</v>
+      </c>
+      <c r="I23" s="25">
+        <v>0</v>
+      </c>
+      <c r="J23" s="25">
+        <v>47</v>
+      </c>
+      <c r="K23" s="25">
+        <v>56</v>
+      </c>
+      <c r="L23" s="25">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A24" s="25" t="s">
+        <v>130</v>
+      </c>
+      <c r="B24" s="25">
+        <v>10</v>
+      </c>
+      <c r="C24" s="25">
+        <v>0</v>
+      </c>
+      <c r="D24" s="25">
+        <v>0</v>
+      </c>
+      <c r="E24" s="25">
+        <v>0</v>
+      </c>
+      <c r="F24" s="25">
+        <v>0</v>
+      </c>
+      <c r="G24" s="25">
+        <v>3</v>
+      </c>
+      <c r="H24" s="25">
+        <v>0</v>
+      </c>
+      <c r="I24" s="25">
+        <v>0</v>
+      </c>
+      <c r="J24" s="25">
+        <v>40</v>
+      </c>
+      <c r="K24" s="25">
+        <v>50</v>
+      </c>
+      <c r="L24" s="25">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A25" s="25" t="s">
+        <v>131</v>
+      </c>
+      <c r="B25" s="25">
+        <v>10</v>
+      </c>
+      <c r="C25" s="25">
+        <v>0</v>
+      </c>
+      <c r="D25" s="25">
+        <v>0</v>
+      </c>
+      <c r="E25" s="25">
+        <v>0</v>
+      </c>
+      <c r="F25" s="25">
+        <v>0</v>
+      </c>
+      <c r="G25" s="25">
+        <v>2</v>
+      </c>
+      <c r="H25" s="25">
+        <v>0</v>
+      </c>
+      <c r="I25" s="25">
+        <v>0</v>
+      </c>
+      <c r="J25" s="25">
+        <v>40</v>
+      </c>
+      <c r="K25" s="25">
+        <v>50</v>
+      </c>
+      <c r="L25" s="25">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A26" s="25" t="s">
+        <v>132</v>
+      </c>
+      <c r="B26" s="25">
+        <v>12</v>
+      </c>
+      <c r="C26" s="25">
+        <v>0</v>
+      </c>
+      <c r="D26" s="25">
+        <v>0</v>
+      </c>
+      <c r="E26" s="25">
+        <v>0</v>
+      </c>
+      <c r="F26" s="25">
+        <v>0</v>
+      </c>
+      <c r="G26" s="25">
+        <v>1</v>
+      </c>
+      <c r="H26" s="25">
+        <v>0</v>
+      </c>
+      <c r="I26" s="25">
+        <v>0</v>
+      </c>
+      <c r="J26" s="25">
+        <v>38</v>
+      </c>
+      <c r="K26" s="25">
+        <v>50</v>
+      </c>
+      <c r="L26" s="25">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A27" s="25" t="s">
+        <v>133</v>
+      </c>
+      <c r="B27" s="25">
+        <v>18</v>
+      </c>
+      <c r="C27" s="25">
+        <v>0</v>
+      </c>
+      <c r="D27" s="25">
+        <v>2</v>
+      </c>
+      <c r="E27" s="25">
+        <v>0</v>
+      </c>
+      <c r="F27" s="25">
+        <v>0</v>
+      </c>
+      <c r="G27" s="25">
+        <v>3</v>
+      </c>
+      <c r="H27" s="25">
+        <v>0</v>
+      </c>
+      <c r="I27" s="25">
+        <v>0</v>
+      </c>
+      <c r="J27" s="25">
+        <v>30</v>
+      </c>
+      <c r="K27" s="25">
+        <v>50</v>
+      </c>
+      <c r="L27" s="25">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A28" s="25" t="s">
+        <v>134</v>
+      </c>
+      <c r="B28" s="25">
+        <v>10</v>
+      </c>
+      <c r="C28" s="25">
+        <v>0</v>
+      </c>
+      <c r="D28" s="25">
+        <v>2</v>
+      </c>
+      <c r="E28" s="25">
+        <v>0</v>
+      </c>
+      <c r="F28" s="25">
+        <v>0</v>
+      </c>
+      <c r="G28" s="25">
+        <v>1</v>
+      </c>
+      <c r="H28" s="25">
+        <v>0</v>
+      </c>
+      <c r="I28" s="25">
+        <v>0</v>
+      </c>
+      <c r="J28" s="25">
+        <v>38</v>
+      </c>
+      <c r="K28" s="25">
+        <v>50</v>
+      </c>
+      <c r="L28" s="25">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A29" s="25" t="s">
+        <v>135</v>
+      </c>
+      <c r="B29" s="25">
+        <v>14</v>
+      </c>
+      <c r="C29" s="25">
+        <v>0</v>
+      </c>
+      <c r="D29" s="25">
+        <v>0</v>
+      </c>
+      <c r="E29" s="25">
+        <v>0</v>
+      </c>
+      <c r="F29" s="25">
+        <v>0</v>
+      </c>
+      <c r="G29" s="25">
+        <v>2</v>
+      </c>
+      <c r="H29" s="25">
+        <v>0</v>
+      </c>
+      <c r="I29" s="25">
+        <v>0</v>
+      </c>
+      <c r="J29" s="25">
+        <v>36</v>
+      </c>
+      <c r="K29" s="25">
+        <v>50</v>
+      </c>
+      <c r="L29" s="25">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A30" s="25" t="s">
+        <v>136</v>
+      </c>
+      <c r="B30" s="25">
+        <v>8</v>
+      </c>
+      <c r="C30" s="25">
+        <v>0</v>
+      </c>
+      <c r="D30" s="25">
+        <v>0</v>
+      </c>
+      <c r="E30" s="25">
+        <v>0</v>
+      </c>
+      <c r="F30" s="25">
+        <v>1</v>
+      </c>
+      <c r="G30" s="25">
+        <v>3</v>
+      </c>
+      <c r="H30" s="25">
+        <v>0</v>
+      </c>
+      <c r="I30" s="25">
+        <v>0</v>
+      </c>
+      <c r="J30" s="25">
+        <v>20</v>
+      </c>
+      <c r="K30" s="25">
+        <v>29</v>
+      </c>
+      <c r="L30" s="25">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A31" s="25" t="s">
+        <v>137</v>
+      </c>
+      <c r="B31" s="25">
+        <v>12</v>
+      </c>
+      <c r="C31" s="25">
+        <v>0</v>
+      </c>
+      <c r="D31" s="25">
+        <v>1</v>
+      </c>
+      <c r="E31" s="25">
+        <v>0</v>
+      </c>
+      <c r="F31" s="25">
+        <v>0</v>
+      </c>
+      <c r="G31" s="25">
+        <v>3</v>
+      </c>
+      <c r="H31" s="25">
+        <v>0</v>
+      </c>
+      <c r="I31" s="25">
+        <v>0</v>
+      </c>
+      <c r="J31" s="25">
+        <v>37</v>
+      </c>
+      <c r="K31" s="25">
+        <v>50</v>
+      </c>
+      <c r="L31" s="25">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A32" s="25" t="s">
+        <v>138</v>
+      </c>
+      <c r="B32" s="25">
+        <v>14</v>
+      </c>
+      <c r="C32" s="25">
+        <v>0</v>
+      </c>
+      <c r="D32" s="25">
+        <v>2</v>
+      </c>
+      <c r="E32" s="25">
+        <v>0</v>
+      </c>
+      <c r="F32" s="25">
+        <v>0</v>
+      </c>
+      <c r="G32" s="25">
+        <v>3</v>
+      </c>
+      <c r="H32" s="25">
+        <v>0</v>
+      </c>
+      <c r="I32" s="25">
+        <v>0</v>
+      </c>
+      <c r="J32" s="25">
+        <v>34</v>
+      </c>
+      <c r="K32" s="25">
+        <v>50</v>
+      </c>
+      <c r="L32" s="25">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A33" s="25" t="s">
+        <v>139</v>
+      </c>
+      <c r="B33" s="25">
+        <v>7</v>
+      </c>
+      <c r="C33" s="25">
+        <v>0</v>
+      </c>
+      <c r="D33" s="25">
+        <v>0</v>
+      </c>
+      <c r="E33" s="25">
+        <v>0</v>
+      </c>
+      <c r="F33" s="25">
+        <v>0</v>
+      </c>
+      <c r="G33" s="25">
+        <v>3</v>
+      </c>
+      <c r="H33" s="25">
+        <v>0</v>
+      </c>
+      <c r="I33" s="25">
+        <v>0</v>
+      </c>
+      <c r="J33" s="25">
+        <v>43</v>
+      </c>
+      <c r="K33" s="25">
+        <v>50</v>
+      </c>
+      <c r="L33" s="25">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A34" s="25" t="s">
+        <v>140</v>
+      </c>
+      <c r="B34" s="25">
+        <v>13</v>
+      </c>
+      <c r="C34" s="25">
+        <v>0</v>
+      </c>
+      <c r="D34" s="25">
+        <v>0</v>
+      </c>
+      <c r="E34" s="25">
+        <v>0</v>
+      </c>
+      <c r="F34" s="25">
+        <v>0</v>
+      </c>
+      <c r="G34" s="25">
+        <v>2</v>
+      </c>
+      <c r="H34" s="25">
+        <v>0</v>
+      </c>
+      <c r="I34" s="25">
+        <v>0</v>
+      </c>
+      <c r="J34" s="25">
+        <v>37</v>
+      </c>
+      <c r="K34" s="25">
+        <v>50</v>
+      </c>
+      <c r="L34" s="25">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="35" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A35" s="25" t="s">
+        <v>141</v>
+      </c>
+      <c r="B35" s="25">
+        <v>10</v>
+      </c>
+      <c r="C35" s="25">
+        <v>0</v>
+      </c>
+      <c r="D35" s="25">
+        <v>0</v>
+      </c>
+      <c r="E35" s="25">
+        <v>0</v>
+      </c>
+      <c r="F35" s="25">
+        <v>1</v>
+      </c>
+      <c r="G35" s="25">
+        <v>4</v>
+      </c>
+      <c r="H35" s="25">
+        <v>0</v>
+      </c>
+      <c r="I35" s="25">
+        <v>0</v>
+      </c>
+      <c r="J35" s="25">
+        <v>25</v>
+      </c>
+      <c r="K35" s="25">
+        <v>36</v>
+      </c>
+      <c r="L35" s="25">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="36" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A36" s="25" t="s">
+        <v>142</v>
+      </c>
+      <c r="B36" s="25">
+        <v>8</v>
+      </c>
+      <c r="C36" s="25">
+        <v>0</v>
+      </c>
+      <c r="D36" s="25">
+        <v>0</v>
+      </c>
+      <c r="E36" s="25">
+        <v>0</v>
+      </c>
+      <c r="F36" s="25">
+        <v>0</v>
+      </c>
+      <c r="G36" s="25">
+        <v>6</v>
+      </c>
+      <c r="H36" s="25">
+        <v>0</v>
+      </c>
+      <c r="I36" s="25">
+        <v>0</v>
+      </c>
+      <c r="J36" s="25">
+        <v>42</v>
+      </c>
+      <c r="K36" s="25">
+        <v>50</v>
+      </c>
+      <c r="L36" s="25">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="37" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A37" s="25" t="s">
+        <v>143</v>
+      </c>
+      <c r="B37" s="25">
+        <v>14</v>
+      </c>
+      <c r="C37" s="25">
+        <v>0</v>
+      </c>
+      <c r="D37" s="25">
+        <v>0</v>
+      </c>
+      <c r="E37" s="25">
+        <v>0</v>
+      </c>
+      <c r="F37" s="25">
+        <v>0</v>
+      </c>
+      <c r="G37" s="25">
+        <v>4</v>
+      </c>
+      <c r="H37" s="25">
+        <v>0</v>
+      </c>
+      <c r="I37" s="25">
+        <v>0</v>
+      </c>
+      <c r="J37" s="25">
+        <v>36</v>
+      </c>
+      <c r="K37" s="25">
+        <v>50</v>
+      </c>
+      <c r="L37" s="25">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="38" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A38" s="25" t="s">
+        <v>144</v>
+      </c>
+      <c r="B38" s="25">
+        <v>11</v>
+      </c>
+      <c r="C38" s="25">
+        <v>0</v>
+      </c>
+      <c r="D38" s="25">
+        <v>0</v>
+      </c>
+      <c r="E38" s="25">
+        <v>0</v>
+      </c>
+      <c r="F38" s="25">
+        <v>0</v>
+      </c>
+      <c r="G38" s="25">
+        <v>3</v>
+      </c>
+      <c r="H38" s="25">
+        <v>0</v>
+      </c>
+      <c r="I38" s="25">
+        <v>0</v>
+      </c>
+      <c r="J38" s="25">
+        <v>39</v>
+      </c>
+      <c r="K38" s="25">
+        <v>50</v>
+      </c>
+      <c r="L38" s="25">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="39" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A39" s="25" t="s">
+        <v>145</v>
+      </c>
+      <c r="B39" s="25">
+        <v>8</v>
+      </c>
+      <c r="C39" s="25">
+        <v>0</v>
+      </c>
+      <c r="D39" s="25">
+        <v>0</v>
+      </c>
+      <c r="E39" s="25">
+        <v>0</v>
+      </c>
+      <c r="F39" s="25">
+        <v>0</v>
+      </c>
+      <c r="G39" s="25">
+        <v>6</v>
+      </c>
+      <c r="H39" s="25">
+        <v>0</v>
+      </c>
+      <c r="I39" s="25">
+        <v>0</v>
+      </c>
+      <c r="J39" s="25">
+        <v>42</v>
+      </c>
+      <c r="K39" s="25">
+        <v>50</v>
+      </c>
+      <c r="L39" s="25">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="40" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A40" s="25" t="s">
+        <v>146</v>
+      </c>
+      <c r="B40" s="25">
+        <v>13</v>
+      </c>
+      <c r="C40" s="25">
+        <v>0</v>
+      </c>
+      <c r="D40" s="25">
+        <v>3</v>
+      </c>
+      <c r="E40" s="25">
+        <v>0</v>
+      </c>
+      <c r="F40" s="25">
+        <v>1</v>
+      </c>
+      <c r="G40" s="25">
+        <v>6</v>
+      </c>
+      <c r="H40" s="25">
+        <v>0</v>
+      </c>
+      <c r="I40" s="25">
+        <v>0</v>
+      </c>
+      <c r="J40" s="25">
+        <v>40</v>
+      </c>
+      <c r="K40" s="25">
+        <v>57</v>
+      </c>
+      <c r="L40" s="25">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="41" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A41" s="25" t="s">
+        <v>147</v>
+      </c>
+      <c r="B41" s="25">
+        <v>9</v>
+      </c>
+      <c r="C41" s="25">
+        <v>0</v>
+      </c>
+      <c r="D41" s="25">
+        <v>0</v>
+      </c>
+      <c r="E41" s="25">
+        <v>0</v>
+      </c>
+      <c r="F41" s="25">
+        <v>0</v>
+      </c>
+      <c r="G41" s="25">
+        <v>6</v>
+      </c>
+      <c r="H41" s="25">
+        <v>0</v>
+      </c>
+      <c r="I41" s="25">
+        <v>0</v>
+      </c>
+      <c r="J41" s="25">
+        <v>41</v>
+      </c>
+      <c r="K41" s="25">
+        <v>50</v>
+      </c>
+      <c r="L41" s="25">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="42" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A42" s="25" t="s">
+        <v>148</v>
+      </c>
+      <c r="B42" s="25">
+        <v>11</v>
+      </c>
+      <c r="C42" s="25">
+        <v>0</v>
+      </c>
+      <c r="D42" s="25">
+        <v>0</v>
+      </c>
+      <c r="E42" s="25">
+        <v>0</v>
+      </c>
+      <c r="F42" s="25">
+        <v>0</v>
+      </c>
+      <c r="G42" s="25">
+        <v>4</v>
+      </c>
+      <c r="H42" s="25">
+        <v>0</v>
+      </c>
+      <c r="I42" s="25">
+        <v>0</v>
+      </c>
+      <c r="J42" s="25">
+        <v>39</v>
+      </c>
+      <c r="K42" s="25">
+        <v>50</v>
+      </c>
+      <c r="L42" s="25">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="43" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A43" s="25" t="s">
+        <v>149</v>
+      </c>
+      <c r="B43" s="25">
+        <v>13</v>
+      </c>
+      <c r="C43" s="25">
+        <v>0</v>
+      </c>
+      <c r="D43" s="25">
+        <v>0</v>
+      </c>
+      <c r="E43" s="25">
+        <v>0</v>
+      </c>
+      <c r="F43" s="25">
+        <v>0</v>
+      </c>
+      <c r="G43" s="25">
+        <v>3</v>
+      </c>
+      <c r="H43" s="25">
+        <v>0</v>
+      </c>
+      <c r="I43" s="25">
+        <v>0</v>
+      </c>
+      <c r="J43" s="25">
+        <v>37</v>
+      </c>
+      <c r="K43" s="25">
+        <v>50</v>
+      </c>
+      <c r="L43" s="25">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="44" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A44" s="25" t="s">
+        <v>150</v>
+      </c>
+      <c r="B44" s="25">
+        <v>13</v>
+      </c>
+      <c r="C44" s="25">
+        <v>0</v>
+      </c>
+      <c r="D44" s="25">
+        <v>0</v>
+      </c>
+      <c r="E44" s="25">
+        <v>0</v>
+      </c>
+      <c r="F44" s="25">
+        <v>0</v>
+      </c>
+      <c r="G44" s="25">
+        <v>5</v>
+      </c>
+      <c r="H44" s="25">
+        <v>0</v>
+      </c>
+      <c r="I44" s="25">
+        <v>0</v>
+      </c>
+      <c r="J44" s="25">
+        <v>37</v>
+      </c>
+      <c r="K44" s="25">
+        <v>50</v>
+      </c>
+      <c r="L44" s="25">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="45" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A45" s="25" t="s">
+        <v>151</v>
+      </c>
+      <c r="B45" s="25">
+        <v>8</v>
+      </c>
+      <c r="C45" s="25">
+        <v>0</v>
+      </c>
+      <c r="D45" s="25">
+        <v>2</v>
+      </c>
+      <c r="E45" s="25">
+        <v>0</v>
+      </c>
+      <c r="F45" s="25">
+        <v>0</v>
+      </c>
+      <c r="G45" s="25">
+        <v>3</v>
+      </c>
+      <c r="H45" s="25">
+        <v>0</v>
+      </c>
+      <c r="I45" s="25">
+        <v>0</v>
+      </c>
+      <c r="J45" s="25">
+        <v>40</v>
+      </c>
+      <c r="K45" s="25">
+        <v>50</v>
+      </c>
+      <c r="L45" s="25">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="46" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A46" s="25" t="s">
+        <v>152</v>
+      </c>
+      <c r="B46" s="25">
+        <v>8</v>
+      </c>
+      <c r="C46" s="25">
+        <v>0</v>
+      </c>
+      <c r="D46" s="25">
+        <v>0</v>
+      </c>
+      <c r="E46" s="25">
+        <v>0</v>
+      </c>
+      <c r="F46" s="25">
+        <v>1</v>
+      </c>
+      <c r="G46" s="25">
+        <v>6</v>
+      </c>
+      <c r="H46" s="25">
+        <v>0</v>
+      </c>
+      <c r="I46" s="25">
+        <v>0</v>
+      </c>
+      <c r="J46" s="25">
+        <v>55</v>
+      </c>
+      <c r="K46" s="25">
+        <v>64</v>
+      </c>
+      <c r="L46" s="25">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="47" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A47" s="25" t="s">
+        <v>153</v>
+      </c>
+      <c r="B47" s="25">
+        <v>7</v>
+      </c>
+      <c r="C47" s="25">
+        <v>0</v>
+      </c>
+      <c r="D47" s="25">
+        <v>0</v>
+      </c>
+      <c r="E47" s="25">
+        <v>0</v>
+      </c>
+      <c r="F47" s="25">
+        <v>0</v>
+      </c>
+      <c r="G47" s="25">
+        <v>4</v>
+      </c>
+      <c r="H47" s="25">
+        <v>0</v>
+      </c>
+      <c r="I47" s="25">
+        <v>0</v>
+      </c>
+      <c r="J47" s="25">
+        <v>43</v>
+      </c>
+      <c r="K47" s="25">
+        <v>50</v>
+      </c>
+      <c r="L47" s="25">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="48" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A48" s="25" t="s">
+        <v>154</v>
+      </c>
+      <c r="B48" s="25">
+        <v>9</v>
+      </c>
+      <c r="C48" s="25">
+        <v>0</v>
+      </c>
+      <c r="D48" s="25">
+        <v>2</v>
+      </c>
+      <c r="E48" s="25">
+        <v>0</v>
+      </c>
+      <c r="F48" s="25">
+        <v>0</v>
+      </c>
+      <c r="G48" s="25">
+        <v>2</v>
+      </c>
+      <c r="H48" s="25">
+        <v>0</v>
+      </c>
+      <c r="I48" s="25">
+        <v>0</v>
+      </c>
+      <c r="J48" s="25">
+        <v>39</v>
+      </c>
+      <c r="K48" s="25">
+        <v>50</v>
+      </c>
+      <c r="L48" s="25">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="49" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A49" s="25" t="s">
+        <v>155</v>
+      </c>
+      <c r="B49" s="25">
+        <v>5</v>
+      </c>
+      <c r="C49" s="25">
+        <v>0</v>
+      </c>
+      <c r="D49" s="25">
+        <v>0</v>
+      </c>
+      <c r="E49" s="25">
+        <v>0</v>
+      </c>
+      <c r="F49" s="25">
+        <v>0</v>
+      </c>
+      <c r="G49" s="25">
+        <v>6</v>
+      </c>
+      <c r="H49" s="25">
+        <v>0</v>
+      </c>
+      <c r="I49" s="25">
+        <v>0</v>
+      </c>
+      <c r="J49" s="25">
+        <v>45</v>
+      </c>
+      <c r="K49" s="25">
+        <v>50</v>
+      </c>
+      <c r="L49" s="25">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="50" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A50" s="25" t="s">
+        <v>156</v>
+      </c>
+      <c r="B50" s="25">
+        <v>1</v>
+      </c>
+      <c r="C50" s="25">
+        <v>0</v>
+      </c>
+      <c r="D50" s="25">
+        <v>0</v>
+      </c>
+      <c r="E50" s="25">
+        <v>0</v>
+      </c>
+      <c r="F50" s="25">
+        <v>0</v>
+      </c>
+      <c r="G50" s="25">
+        <v>3</v>
+      </c>
+      <c r="H50" s="25">
+        <v>0</v>
+      </c>
+      <c r="I50" s="25">
+        <v>0</v>
+      </c>
+      <c r="J50" s="25">
+        <v>49</v>
+      </c>
+      <c r="K50" s="25">
+        <v>50</v>
+      </c>
+      <c r="L50" s="25">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="51" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A51" s="25" t="s">
+        <v>157</v>
+      </c>
+      <c r="B51" s="25">
+        <v>12</v>
+      </c>
+      <c r="C51" s="25">
+        <v>0</v>
+      </c>
+      <c r="D51" s="25">
+        <v>0</v>
+      </c>
+      <c r="E51" s="25">
+        <v>0</v>
+      </c>
+      <c r="F51" s="25">
+        <v>0</v>
+      </c>
+      <c r="G51" s="25">
+        <v>3</v>
+      </c>
+      <c r="H51" s="25">
+        <v>0</v>
+      </c>
+      <c r="I51" s="25">
+        <v>0</v>
+      </c>
+      <c r="J51" s="25">
+        <v>38</v>
+      </c>
+      <c r="K51" s="25">
+        <v>50</v>
+      </c>
+      <c r="L51" s="25">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="52" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A52" s="25" t="s">
+        <v>158</v>
+      </c>
+      <c r="B52" s="25">
+        <v>15</v>
+      </c>
+      <c r="C52" s="25">
+        <v>0</v>
+      </c>
+      <c r="D52" s="25">
+        <v>0</v>
+      </c>
+      <c r="E52" s="25">
+        <v>0</v>
+      </c>
+      <c r="F52" s="25">
+        <v>0</v>
+      </c>
+      <c r="G52" s="25">
+        <v>2</v>
+      </c>
+      <c r="H52" s="25">
+        <v>0</v>
+      </c>
+      <c r="I52" s="25">
+        <v>0</v>
+      </c>
+      <c r="J52" s="25">
+        <v>35</v>
+      </c>
+      <c r="K52" s="25">
+        <v>50</v>
+      </c>
+      <c r="L52" s="25">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="53" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A53" s="25" t="s">
+        <v>159</v>
+      </c>
+      <c r="B53" s="25">
+        <v>5</v>
+      </c>
+      <c r="C53" s="25">
+        <v>0</v>
+      </c>
+      <c r="D53" s="25">
+        <v>1</v>
+      </c>
+      <c r="E53" s="25">
+        <v>0</v>
+      </c>
+      <c r="F53" s="25">
+        <v>1</v>
+      </c>
+      <c r="G53" s="25">
+        <v>1</v>
+      </c>
+      <c r="H53" s="25">
+        <v>0</v>
+      </c>
+      <c r="I53" s="25">
+        <v>0</v>
+      </c>
+      <c r="J53" s="25">
+        <v>30</v>
+      </c>
+      <c r="K53" s="25">
+        <v>37</v>
+      </c>
+      <c r="L53" s="25">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="54" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A54" s="25" t="s">
+        <v>160</v>
+      </c>
+      <c r="B54" s="25">
+        <v>7</v>
+      </c>
+      <c r="C54" s="25">
+        <v>0</v>
+      </c>
+      <c r="D54" s="25">
+        <v>0</v>
+      </c>
+      <c r="E54" s="25">
+        <v>0</v>
+      </c>
+      <c r="F54" s="25">
+        <v>0</v>
+      </c>
+      <c r="G54" s="25">
+        <v>5</v>
+      </c>
+      <c r="H54" s="25">
+        <v>0</v>
+      </c>
+      <c r="I54" s="25">
+        <v>0</v>
+      </c>
+      <c r="J54" s="25">
+        <v>43</v>
+      </c>
+      <c r="K54" s="25">
+        <v>50</v>
+      </c>
+      <c r="L54" s="25">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="55" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A55" s="25" t="s">
+        <v>161</v>
+      </c>
+      <c r="B55" s="25">
+        <v>11</v>
+      </c>
+      <c r="C55" s="25">
+        <v>0</v>
+      </c>
+      <c r="D55" s="25">
+        <v>2</v>
+      </c>
+      <c r="E55" s="25">
+        <v>0</v>
+      </c>
+      <c r="F55" s="25">
+        <v>0</v>
+      </c>
+      <c r="G55" s="25">
+        <v>1</v>
+      </c>
+      <c r="H55" s="25">
+        <v>0</v>
+      </c>
+      <c r="I55" s="25">
+        <v>0</v>
+      </c>
+      <c r="J55" s="25">
+        <v>37</v>
+      </c>
+      <c r="K55" s="25">
+        <v>50</v>
+      </c>
+      <c r="L55" s="25">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="56" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A56" s="25" t="s">
+        <v>162</v>
+      </c>
+      <c r="B56" s="25">
+        <v>10</v>
+      </c>
+      <c r="C56" s="25">
+        <v>0</v>
+      </c>
+      <c r="D56" s="25">
+        <v>0</v>
+      </c>
+      <c r="E56" s="25">
+        <v>0</v>
+      </c>
+      <c r="F56" s="25">
+        <v>0</v>
+      </c>
+      <c r="G56" s="25">
+        <v>3</v>
+      </c>
+      <c r="H56" s="25">
+        <v>0</v>
+      </c>
+      <c r="I56" s="25">
+        <v>0</v>
+      </c>
+      <c r="J56" s="25">
+        <v>40</v>
+      </c>
+      <c r="K56" s="25">
+        <v>50</v>
+      </c>
+      <c r="L56" s="25">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="57" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A57" s="25" t="s">
+        <v>163</v>
+      </c>
+      <c r="B57" s="25">
+        <v>7</v>
+      </c>
+      <c r="C57" s="25">
+        <v>0</v>
+      </c>
+      <c r="D57" s="25">
+        <v>0</v>
+      </c>
+      <c r="E57" s="25">
+        <v>0</v>
+      </c>
+      <c r="F57" s="25">
+        <v>0</v>
+      </c>
+      <c r="G57" s="25">
+        <v>4</v>
+      </c>
+      <c r="H57" s="25">
+        <v>0</v>
+      </c>
+      <c r="I57" s="25">
+        <v>0</v>
+      </c>
+      <c r="J57" s="25">
+        <v>43</v>
+      </c>
+      <c r="K57" s="25">
+        <v>50</v>
+      </c>
+      <c r="L57" s="25">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="58" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A58" s="25" t="s">
+        <v>164</v>
+      </c>
+      <c r="B58" s="25">
+        <v>9</v>
+      </c>
+      <c r="C58" s="25">
+        <v>0</v>
+      </c>
+      <c r="D58" s="25">
+        <v>0</v>
+      </c>
+      <c r="E58" s="25">
+        <v>0</v>
+      </c>
+      <c r="F58" s="25">
+        <v>1</v>
+      </c>
+      <c r="G58" s="25">
+        <v>2</v>
+      </c>
+      <c r="H58" s="25">
+        <v>0</v>
+      </c>
+      <c r="I58" s="25">
+        <v>0</v>
+      </c>
+      <c r="J58" s="25">
+        <v>52</v>
+      </c>
+      <c r="K58" s="25">
+        <v>62</v>
+      </c>
+      <c r="L58" s="25">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="59" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A59" s="25" t="s">
+        <v>165</v>
+      </c>
+      <c r="B59" s="25">
+        <v>14</v>
+      </c>
+      <c r="C59" s="25">
+        <v>0</v>
+      </c>
+      <c r="D59" s="25">
+        <v>0</v>
+      </c>
+      <c r="E59" s="25">
+        <v>0</v>
+      </c>
+      <c r="F59" s="25">
+        <v>0</v>
+      </c>
+      <c r="G59" s="25">
+        <v>6</v>
+      </c>
+      <c r="H59" s="25">
+        <v>0</v>
+      </c>
+      <c r="I59" s="25">
+        <v>0</v>
+      </c>
+      <c r="J59" s="25">
+        <v>36</v>
+      </c>
+      <c r="K59" s="25">
+        <v>50</v>
+      </c>
+      <c r="L59" s="25">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="60" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A60" s="25" t="s">
+        <v>166</v>
+      </c>
+      <c r="B60" s="25">
+        <v>10</v>
+      </c>
+      <c r="C60" s="25">
+        <v>0</v>
+      </c>
+      <c r="D60" s="25">
+        <v>0</v>
+      </c>
+      <c r="E60" s="25">
+        <v>0</v>
+      </c>
+      <c r="F60" s="25">
+        <v>0</v>
+      </c>
+      <c r="G60" s="25">
+        <v>3</v>
+      </c>
+      <c r="H60" s="25">
+        <v>0</v>
+      </c>
+      <c r="I60" s="25">
+        <v>0</v>
+      </c>
+      <c r="J60" s="25">
+        <v>40</v>
+      </c>
+      <c r="K60" s="25">
+        <v>50</v>
+      </c>
+      <c r="L60" s="25">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="61" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A61" s="25" t="s">
+        <v>167</v>
+      </c>
+      <c r="B61" s="25">
+        <v>13</v>
+      </c>
+      <c r="C61" s="25">
+        <v>0</v>
+      </c>
+      <c r="D61" s="25">
+        <v>0</v>
+      </c>
+      <c r="E61" s="25">
+        <v>0</v>
+      </c>
+      <c r="F61" s="25">
+        <v>0</v>
+      </c>
+      <c r="G61" s="25">
+        <v>5</v>
+      </c>
+      <c r="H61" s="25">
+        <v>0</v>
+      </c>
+      <c r="I61" s="25">
+        <v>0</v>
+      </c>
+      <c r="J61" s="25">
+        <v>37</v>
+      </c>
+      <c r="K61" s="25">
+        <v>50</v>
+      </c>
+      <c r="L61" s="25">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="62" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A62" s="25" t="s">
+        <v>168</v>
+      </c>
+      <c r="B62" s="25">
+        <v>9</v>
+      </c>
+      <c r="C62" s="25">
+        <v>0</v>
+      </c>
+      <c r="D62" s="25">
+        <v>2</v>
+      </c>
+      <c r="E62" s="25">
+        <v>0</v>
+      </c>
+      <c r="F62" s="25">
+        <v>0</v>
+      </c>
+      <c r="G62" s="25">
+        <v>4</v>
+      </c>
+      <c r="H62" s="25">
+        <v>0</v>
+      </c>
+      <c r="I62" s="25">
+        <v>0</v>
+      </c>
+      <c r="J62" s="25">
+        <v>39</v>
+      </c>
+      <c r="K62" s="25">
+        <v>50</v>
+      </c>
+      <c r="L62" s="25">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="63" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A63" s="25" t="s">
+        <v>169</v>
+      </c>
+      <c r="B63" s="25">
+        <v>12</v>
+      </c>
+      <c r="C63" s="25">
+        <v>0</v>
+      </c>
+      <c r="D63" s="25">
+        <v>0</v>
+      </c>
+      <c r="E63" s="25">
+        <v>0</v>
+      </c>
+      <c r="F63" s="25">
+        <v>0</v>
+      </c>
+      <c r="G63" s="25">
+        <v>4</v>
+      </c>
+      <c r="H63" s="25">
+        <v>0</v>
+      </c>
+      <c r="I63" s="25">
+        <v>0</v>
+      </c>
+      <c r="J63" s="25">
+        <v>38</v>
+      </c>
+      <c r="K63" s="25">
+        <v>50</v>
+      </c>
+      <c r="L63" s="25">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="64" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A64" s="25" t="s">
+        <v>170</v>
+      </c>
+      <c r="B64" s="25">
+        <v>13</v>
+      </c>
+      <c r="C64" s="25">
+        <v>0</v>
+      </c>
+      <c r="D64" s="25">
+        <v>0</v>
+      </c>
+      <c r="E64" s="25">
+        <v>0</v>
+      </c>
+      <c r="F64" s="25">
+        <v>1</v>
+      </c>
+      <c r="G64" s="25">
+        <v>4</v>
+      </c>
+      <c r="H64" s="25">
+        <v>0</v>
+      </c>
+      <c r="I64" s="25">
+        <v>0</v>
+      </c>
+      <c r="J64" s="25">
+        <v>50</v>
+      </c>
+      <c r="K64" s="25">
+        <v>64</v>
+      </c>
+      <c r="L64" s="25">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="65" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A65" s="25" t="s">
+        <v>171</v>
+      </c>
+      <c r="B65" s="25">
+        <v>5</v>
+      </c>
+      <c r="C65" s="25">
+        <v>3</v>
+      </c>
+      <c r="D65" s="25">
+        <v>0</v>
+      </c>
+      <c r="E65" s="25">
+        <v>0</v>
+      </c>
+      <c r="F65" s="25">
+        <v>6</v>
+      </c>
+      <c r="G65" s="25">
+        <v>3</v>
+      </c>
+      <c r="H65" s="25">
+        <v>0</v>
+      </c>
+      <c r="I65" s="25">
+        <v>0</v>
+      </c>
+      <c r="J65" s="25">
+        <v>42</v>
+      </c>
+      <c r="K65" s="25">
+        <v>50</v>
+      </c>
+      <c r="L65" s="25">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="66" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A66" s="25" t="s">
+        <v>172</v>
+      </c>
+      <c r="B66" s="25">
+        <v>5</v>
+      </c>
+      <c r="C66" s="25">
+        <v>0</v>
+      </c>
+      <c r="D66" s="25">
+        <v>0</v>
+      </c>
+      <c r="E66" s="25">
+        <v>0</v>
+      </c>
+      <c r="F66" s="25">
+        <v>7</v>
+      </c>
+      <c r="G66" s="25">
+        <v>2</v>
+      </c>
+      <c r="H66" s="25">
+        <v>0</v>
+      </c>
+      <c r="I66" s="25">
+        <v>0</v>
+      </c>
+      <c r="J66" s="25">
+        <v>38</v>
+      </c>
+      <c r="K66" s="25">
+        <v>50</v>
+      </c>
+      <c r="L66" s="25">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="67" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A67" s="25" t="s">
+        <v>173</v>
+      </c>
+      <c r="B67" s="25">
+        <v>9</v>
+      </c>
+      <c r="C67" s="25">
+        <v>1</v>
+      </c>
+      <c r="D67" s="25">
+        <v>1</v>
+      </c>
+      <c r="E67" s="25">
+        <v>0</v>
+      </c>
+      <c r="F67" s="25">
+        <v>7</v>
+      </c>
+      <c r="G67" s="25">
+        <v>3</v>
+      </c>
+      <c r="H67" s="25">
+        <v>0</v>
+      </c>
+      <c r="I67" s="25">
+        <v>0</v>
+      </c>
+      <c r="J67" s="25">
+        <v>34</v>
+      </c>
+      <c r="K67" s="25">
+        <v>50</v>
+      </c>
+      <c r="L67" s="25">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="68" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A68" s="25" t="s">
+        <v>174</v>
+      </c>
+      <c r="B68" s="25">
+        <v>6</v>
+      </c>
+      <c r="C68" s="25">
+        <v>0</v>
+      </c>
+      <c r="D68" s="25">
+        <v>0</v>
+      </c>
+      <c r="E68" s="25">
+        <v>0</v>
+      </c>
+      <c r="F68" s="25">
+        <v>5</v>
+      </c>
+      <c r="G68" s="25">
+        <v>1</v>
+      </c>
+      <c r="H68" s="25">
+        <v>0</v>
+      </c>
+      <c r="I68" s="25">
+        <v>0</v>
+      </c>
+      <c r="J68" s="25">
+        <v>39</v>
+      </c>
+      <c r="K68" s="25">
+        <v>50</v>
+      </c>
+      <c r="L68" s="25">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="69" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A69" s="25" t="s">
+        <v>175</v>
+      </c>
+      <c r="B69" s="25">
+        <v>7</v>
+      </c>
+      <c r="C69" s="25">
+        <v>0</v>
+      </c>
+      <c r="D69" s="25">
+        <v>1</v>
+      </c>
+      <c r="E69" s="25">
+        <v>0</v>
+      </c>
+      <c r="F69" s="25">
+        <v>5</v>
+      </c>
+      <c r="G69" s="25">
+        <v>3</v>
+      </c>
+      <c r="H69" s="25">
+        <v>0</v>
+      </c>
+      <c r="I69" s="25">
+        <v>0</v>
+      </c>
+      <c r="J69" s="25">
+        <v>37</v>
+      </c>
+      <c r="K69" s="25">
+        <v>50</v>
+      </c>
+      <c r="L69" s="25">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="70" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A70" s="25" t="s">
+        <v>176</v>
+      </c>
+      <c r="B70" s="25">
+        <v>6</v>
+      </c>
+      <c r="C70" s="25">
+        <v>3</v>
+      </c>
+      <c r="D70" s="25">
+        <v>2</v>
+      </c>
+      <c r="E70" s="25">
+        <v>0</v>
+      </c>
+      <c r="F70" s="25">
+        <v>6</v>
+      </c>
+      <c r="G70" s="25">
+        <v>3</v>
+      </c>
+      <c r="H70" s="25">
+        <v>0</v>
+      </c>
+      <c r="I70" s="25">
+        <v>0</v>
+      </c>
+      <c r="J70" s="25">
+        <v>39</v>
+      </c>
+      <c r="K70" s="25">
+        <v>50</v>
+      </c>
+      <c r="L70" s="25">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="71" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A71" s="25" t="s">
+        <v>177</v>
+      </c>
+      <c r="B71" s="25">
+        <v>3</v>
+      </c>
+      <c r="C71" s="25">
+        <v>1</v>
+      </c>
+      <c r="D71" s="25">
+        <v>4</v>
+      </c>
+      <c r="E71" s="25">
+        <v>0</v>
+      </c>
+      <c r="F71" s="25">
+        <v>7</v>
+      </c>
+      <c r="G71" s="25">
+        <v>5</v>
+      </c>
+      <c r="H71" s="25">
+        <v>0</v>
+      </c>
+      <c r="I71" s="25">
+        <v>1</v>
+      </c>
+      <c r="J71" s="25">
+        <v>37</v>
+      </c>
+      <c r="K71" s="25">
+        <v>50</v>
+      </c>
+      <c r="L71" s="25">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="72" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A72" s="25" t="s">
+        <v>178</v>
+      </c>
+      <c r="B72" s="25">
+        <v>8</v>
+      </c>
+      <c r="C72" s="25">
+        <v>2</v>
+      </c>
+      <c r="D72" s="25">
+        <v>0</v>
+      </c>
+      <c r="E72" s="25">
+        <v>0</v>
+      </c>
+      <c r="F72" s="25">
+        <v>6</v>
+      </c>
+      <c r="G72" s="25">
+        <v>3</v>
+      </c>
+      <c r="H72" s="25">
+        <v>0</v>
+      </c>
+      <c r="I72" s="25">
+        <v>1</v>
+      </c>
+      <c r="J72" s="25">
+        <v>28</v>
+      </c>
+      <c r="K72" s="25">
+        <v>40</v>
+      </c>
+      <c r="L72" s="25">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="73" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A73" s="27" t="s">
+        <v>179</v>
+      </c>
+      <c r="B73" s="28">
+        <f>SUM(B2:B72)</f>
+        <v>681</v>
+      </c>
+      <c r="C73" s="28">
+        <f t="shared" ref="C73:L73" si="0">SUM(C2:C72)</f>
+        <v>11</v>
+      </c>
+      <c r="D73" s="28">
+        <f t="shared" si="0"/>
+        <v>38</v>
+      </c>
+      <c r="E73" s="28">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F73" s="28">
+        <f t="shared" si="0"/>
+        <v>61</v>
+      </c>
+      <c r="G73" s="28">
+        <f t="shared" si="0"/>
+        <v>264</v>
+      </c>
+      <c r="H73" s="28">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I73" s="28">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="J73" s="28">
+        <f t="shared" si="0"/>
+        <v>2757</v>
+      </c>
+      <c r="K73" s="28">
+        <f t="shared" si="0"/>
+        <v>3526</v>
+      </c>
+      <c r="L73" s="28">
+        <f t="shared" si="0"/>
+        <v>4234</v>
+      </c>
+    </row>
+    <row r="74" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B74" s="3"/>
+      <c r="C74" s="3"/>
+      <c r="D74" s="3"/>
+      <c r="E74" t="s">
+        <v>12</v>
+      </c>
+      <c r="F74">
+        <f>G73</f>
+        <v>264</v>
+      </c>
+      <c r="J74">
+        <f>B73-C73</f>
+        <v>670</v>
+      </c>
+      <c r="K74" s="3"/>
+      <c r="L74" s="3"/>
+    </row>
+    <row r="75" spans="1:12" ht="18" x14ac:dyDescent="0.25">
+      <c r="A75" s="26"/>
+      <c r="C75" s="24"/>
+      <c r="D75" s="24"/>
+      <c r="E75" t="s">
+        <v>13</v>
+      </c>
+      <c r="F75">
+        <f>B73</f>
+        <v>681</v>
+      </c>
+      <c r="J75">
+        <f>D73-E73</f>
+        <v>38</v>
+      </c>
+      <c r="K75" s="24"/>
+    </row>
+    <row r="76" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="E76" t="s">
+        <v>14</v>
+      </c>
+      <c r="F76">
+        <v>22</v>
+      </c>
+      <c r="J76">
+        <f>F82</f>
+        <v>3526</v>
+      </c>
+    </row>
+    <row r="77" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="E77" t="s">
+        <v>15</v>
+      </c>
+      <c r="F77">
+        <v>16</v>
+      </c>
+      <c r="J77" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="78" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="F78" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="J78">
+        <f>SUM(J74:J77)</f>
+        <v>4234</v>
+      </c>
+    </row>
+    <row r="79" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="F79">
+        <f>SUM(F74:F78)</f>
+        <v>983</v>
+      </c>
+      <c r="J79" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="80" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="F80">
+        <f>K73-F79</f>
+        <v>2543</v>
+      </c>
+      <c r="J80">
+        <f>J78-L73</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F81" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="82" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F82">
+        <f>F80+F79</f>
+        <v>3526</v>
+      </c>
+    </row>
+    <row r="83" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F83">
+        <f>F82-K73</f>
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:K9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A7" workbookViewId="0">
       <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
nmv 28 05 2022
</commit_message>
<xml_diff>
--- a/TS Jatai Ghanam Project/Stas table for TS 2.1 TO 2.6.xlsx
+++ b/TS Jatai Ghanam Project/Stas table for TS 2.1 TO 2.6.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7095" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7095"/>
   </bookViews>
   <sheets>
     <sheet name="TS 2.1" sheetId="8" r:id="rId1"/>
@@ -2018,7 +2018,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
@@ -2100,6 +2100,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -2384,15 +2387,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M77"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A65" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E68" sqref="E68:J77"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A62" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="R62" sqref="R62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="4.85546875" customWidth="1"/>
+    <col min="2" max="2" width="6.5703125" customWidth="1"/>
     <col min="3" max="3" width="7.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="4.42578125" customWidth="1"/>
     <col min="5" max="5" width="7.42578125" bestFit="1" customWidth="1"/>
@@ -2460,7 +2463,7 @@
       <c r="F2" s="4">
         <v>0</v>
       </c>
-      <c r="G2" s="4">
+      <c r="G2" s="31">
         <v>4</v>
       </c>
       <c r="H2" s="4">
@@ -2499,7 +2502,7 @@
       <c r="F3" s="4">
         <v>0</v>
       </c>
-      <c r="G3" s="4">
+      <c r="G3" s="31">
         <v>4</v>
       </c>
       <c r="H3" s="4">
@@ -2538,7 +2541,7 @@
       <c r="F4" s="4">
         <v>0</v>
       </c>
-      <c r="G4" s="4">
+      <c r="G4" s="31">
         <v>6</v>
       </c>
       <c r="H4" s="4">
@@ -2577,8 +2580,8 @@
       <c r="F5" s="4">
         <v>0</v>
       </c>
-      <c r="G5" s="4">
-        <v>3</v>
+      <c r="G5" s="31">
+        <v>4</v>
       </c>
       <c r="H5" s="4">
         <v>0</v>
@@ -2616,7 +2619,7 @@
       <c r="F6" s="4">
         <v>0</v>
       </c>
-      <c r="G6" s="4">
+      <c r="G6" s="31">
         <v>3</v>
       </c>
       <c r="H6" s="4">
@@ -2655,8 +2658,8 @@
       <c r="F7" s="4">
         <v>1</v>
       </c>
-      <c r="G7" s="4">
-        <v>6</v>
+      <c r="G7" s="31">
+        <v>7</v>
       </c>
       <c r="H7" s="4">
         <v>0</v>
@@ -2694,7 +2697,7 @@
       <c r="F8" s="4">
         <v>0</v>
       </c>
-      <c r="G8" s="4">
+      <c r="G8" s="31">
         <v>3</v>
       </c>
       <c r="H8" s="4">
@@ -2733,7 +2736,7 @@
       <c r="F9" s="4">
         <v>0</v>
       </c>
-      <c r="G9" s="4">
+      <c r="G9" s="31">
         <v>1</v>
       </c>
       <c r="H9" s="4">
@@ -2772,7 +2775,7 @@
       <c r="F10" s="4">
         <v>0</v>
       </c>
-      <c r="G10" s="4">
+      <c r="G10" s="31">
         <v>5</v>
       </c>
       <c r="H10" s="4">
@@ -2811,7 +2814,7 @@
       <c r="F11" s="4">
         <v>0</v>
       </c>
-      <c r="G11" s="4">
+      <c r="G11" s="31">
         <v>6</v>
       </c>
       <c r="H11" s="4">
@@ -2850,7 +2853,7 @@
       <c r="F12" s="4">
         <v>0</v>
       </c>
-      <c r="G12" s="4">
+      <c r="G12" s="31">
         <v>2</v>
       </c>
       <c r="H12" s="4">
@@ -2889,8 +2892,8 @@
       <c r="F13" s="4">
         <v>0</v>
       </c>
-      <c r="G13" s="4">
-        <v>3</v>
+      <c r="G13" s="31">
+        <v>4</v>
       </c>
       <c r="H13" s="4">
         <v>0</v>
@@ -2928,7 +2931,7 @@
       <c r="F14" s="4">
         <v>0</v>
       </c>
-      <c r="G14" s="4">
+      <c r="G14" s="31">
         <v>2</v>
       </c>
       <c r="H14" s="4">
@@ -2967,7 +2970,7 @@
       <c r="F15" s="4">
         <v>0</v>
       </c>
-      <c r="G15" s="4">
+      <c r="G15" s="31">
         <v>3</v>
       </c>
       <c r="H15" s="4">
@@ -3006,7 +3009,7 @@
       <c r="F16" s="4">
         <v>1</v>
       </c>
-      <c r="G16" s="4">
+      <c r="G16" s="31">
         <v>2</v>
       </c>
       <c r="H16" s="4">
@@ -3045,7 +3048,7 @@
       <c r="F17" s="4">
         <v>0</v>
       </c>
-      <c r="G17" s="4">
+      <c r="G17" s="31">
         <v>6</v>
       </c>
       <c r="H17" s="4">
@@ -3084,7 +3087,7 @@
       <c r="F18" s="4">
         <v>0</v>
       </c>
-      <c r="G18" s="4">
+      <c r="G18" s="31">
         <v>4</v>
       </c>
       <c r="H18" s="4">
@@ -3123,7 +3126,7 @@
       <c r="F19" s="4">
         <v>0</v>
       </c>
-      <c r="G19" s="4">
+      <c r="G19" s="31">
         <v>4</v>
       </c>
       <c r="H19" s="4">
@@ -3162,7 +3165,7 @@
       <c r="F20" s="4">
         <v>0</v>
       </c>
-      <c r="G20" s="4">
+      <c r="G20" s="31">
         <v>5</v>
       </c>
       <c r="H20" s="4">
@@ -3201,7 +3204,7 @@
       <c r="F21" s="4">
         <v>1</v>
       </c>
-      <c r="G21" s="4">
+      <c r="G21" s="31">
         <v>6</v>
       </c>
       <c r="H21" s="4">
@@ -3240,8 +3243,8 @@
       <c r="F22" s="4">
         <v>0</v>
       </c>
-      <c r="G22" s="4">
-        <v>4</v>
+      <c r="G22" s="31">
+        <v>5</v>
       </c>
       <c r="H22" s="4">
         <v>0</v>
@@ -3279,8 +3282,8 @@
       <c r="F23" s="4">
         <v>0</v>
       </c>
-      <c r="G23" s="4">
-        <v>2</v>
+      <c r="G23" s="31">
+        <v>3</v>
       </c>
       <c r="H23" s="4">
         <v>0</v>
@@ -3318,7 +3321,7 @@
       <c r="F24" s="4">
         <v>0</v>
       </c>
-      <c r="G24" s="4">
+      <c r="G24" s="31">
         <v>3</v>
       </c>
       <c r="H24" s="4">
@@ -3357,7 +3360,7 @@
       <c r="F25" s="4">
         <v>0</v>
       </c>
-      <c r="G25" s="4">
+      <c r="G25" s="31">
         <v>4</v>
       </c>
       <c r="H25" s="4">
@@ -3396,8 +3399,8 @@
       <c r="F26" s="4">
         <v>0</v>
       </c>
-      <c r="G26" s="4">
-        <v>3</v>
+      <c r="G26" s="31">
+        <v>6</v>
       </c>
       <c r="H26" s="4">
         <v>0</v>
@@ -3435,7 +3438,7 @@
       <c r="F27" s="4">
         <v>0</v>
       </c>
-      <c r="G27" s="4">
+      <c r="G27" s="31">
         <v>3</v>
       </c>
       <c r="H27" s="4">
@@ -3474,7 +3477,7 @@
       <c r="F28" s="4">
         <v>0</v>
       </c>
-      <c r="G28" s="4">
+      <c r="G28" s="31">
         <v>4</v>
       </c>
       <c r="H28" s="4">
@@ -3513,7 +3516,7 @@
       <c r="F29" s="4">
         <v>1</v>
       </c>
-      <c r="G29" s="4">
+      <c r="G29" s="31">
         <v>5</v>
       </c>
       <c r="H29" s="4">
@@ -3552,8 +3555,8 @@
       <c r="F30" s="4">
         <v>0</v>
       </c>
-      <c r="G30" s="4">
-        <v>6</v>
+      <c r="G30" s="31">
+        <v>8</v>
       </c>
       <c r="H30" s="4">
         <v>0</v>
@@ -3591,8 +3594,8 @@
       <c r="F31" s="4">
         <v>0</v>
       </c>
-      <c r="G31" s="4">
-        <v>3</v>
+      <c r="G31" s="31">
+        <v>4</v>
       </c>
       <c r="H31" s="4">
         <v>0</v>
@@ -3630,8 +3633,8 @@
       <c r="F32" s="4">
         <v>0</v>
       </c>
-      <c r="G32" s="4">
-        <v>4</v>
+      <c r="G32" s="31">
+        <v>5</v>
       </c>
       <c r="H32" s="4">
         <v>0</v>
@@ -3669,7 +3672,7 @@
       <c r="F33" s="4">
         <v>0</v>
       </c>
-      <c r="G33" s="4">
+      <c r="G33" s="31">
         <v>1</v>
       </c>
       <c r="H33" s="4">
@@ -3708,8 +3711,8 @@
       <c r="F34" s="4">
         <v>0</v>
       </c>
-      <c r="G34" s="4">
-        <v>5</v>
+      <c r="G34" s="31">
+        <v>6</v>
       </c>
       <c r="H34" s="4">
         <v>0</v>
@@ -3747,8 +3750,8 @@
       <c r="F35" s="4">
         <v>0</v>
       </c>
-      <c r="G35" s="4">
-        <v>4</v>
+      <c r="G35" s="31">
+        <v>6</v>
       </c>
       <c r="H35" s="4">
         <v>0</v>
@@ -3786,7 +3789,7 @@
       <c r="F36" s="4">
         <v>1</v>
       </c>
-      <c r="G36" s="4">
+      <c r="G36" s="31">
         <v>5</v>
       </c>
       <c r="H36" s="4">
@@ -3825,7 +3828,7 @@
       <c r="F37" s="4">
         <v>0</v>
       </c>
-      <c r="G37" s="4">
+      <c r="G37" s="31">
         <v>4</v>
       </c>
       <c r="H37" s="4">
@@ -3864,7 +3867,7 @@
       <c r="F38" s="4">
         <v>0</v>
       </c>
-      <c r="G38" s="4">
+      <c r="G38" s="31">
         <v>5</v>
       </c>
       <c r="H38" s="4">
@@ -3903,7 +3906,7 @@
       <c r="F39" s="4">
         <v>0</v>
       </c>
-      <c r="G39" s="4">
+      <c r="G39" s="31">
         <v>4</v>
       </c>
       <c r="H39" s="4">
@@ -3942,7 +3945,7 @@
       <c r="F40" s="4">
         <v>0</v>
       </c>
-      <c r="G40" s="4">
+      <c r="G40" s="31">
         <v>5</v>
       </c>
       <c r="H40" s="4">
@@ -3981,7 +3984,7 @@
       <c r="F41" s="4">
         <v>1</v>
       </c>
-      <c r="G41" s="4">
+      <c r="G41" s="31">
         <v>3</v>
       </c>
       <c r="H41" s="4">
@@ -4020,7 +4023,7 @@
       <c r="F42" s="4">
         <v>0</v>
       </c>
-      <c r="G42" s="4">
+      <c r="G42" s="31">
         <v>6</v>
       </c>
       <c r="H42" s="4">
@@ -4059,7 +4062,7 @@
       <c r="F43" s="4">
         <v>0</v>
       </c>
-      <c r="G43" s="4">
+      <c r="G43" s="31">
         <v>4</v>
       </c>
       <c r="H43" s="4">
@@ -4098,8 +4101,8 @@
       <c r="F44" s="4">
         <v>0</v>
       </c>
-      <c r="G44" s="4">
-        <v>2</v>
+      <c r="G44" s="31">
+        <v>3</v>
       </c>
       <c r="H44" s="4">
         <v>0</v>
@@ -4137,8 +4140,8 @@
       <c r="F45" s="4">
         <v>0</v>
       </c>
-      <c r="G45" s="4">
-        <v>4</v>
+      <c r="G45" s="31">
+        <v>6</v>
       </c>
       <c r="H45" s="4">
         <v>0</v>
@@ -4176,8 +4179,8 @@
       <c r="F46" s="4">
         <v>0</v>
       </c>
-      <c r="G46" s="4">
-        <v>4</v>
+      <c r="G46" s="31">
+        <v>5</v>
       </c>
       <c r="H46" s="4">
         <v>0</v>
@@ -4215,8 +4218,8 @@
       <c r="F47" s="4">
         <v>0</v>
       </c>
-      <c r="G47" s="4">
-        <v>4</v>
+      <c r="G47" s="31">
+        <v>5</v>
       </c>
       <c r="H47" s="4">
         <v>0</v>
@@ -4254,8 +4257,8 @@
       <c r="F48" s="4">
         <v>1</v>
       </c>
-      <c r="G48" s="4">
-        <v>5</v>
+      <c r="G48" s="31">
+        <v>6</v>
       </c>
       <c r="H48" s="4">
         <v>0</v>
@@ -4293,8 +4296,8 @@
       <c r="F49" s="4">
         <v>0</v>
       </c>
-      <c r="G49" s="4">
-        <v>3</v>
+      <c r="G49" s="31">
+        <v>4</v>
       </c>
       <c r="H49" s="4">
         <v>0</v>
@@ -4332,8 +4335,8 @@
       <c r="F50" s="4">
         <v>0</v>
       </c>
-      <c r="G50" s="4">
-        <v>3</v>
+      <c r="G50" s="31">
+        <v>5</v>
       </c>
       <c r="H50" s="4">
         <v>0</v>
@@ -4371,7 +4374,7 @@
       <c r="F51" s="4">
         <v>0</v>
       </c>
-      <c r="G51" s="4">
+      <c r="G51" s="31">
         <v>5</v>
       </c>
       <c r="H51" s="4">
@@ -4410,8 +4413,8 @@
       <c r="F52" s="4">
         <v>0</v>
       </c>
-      <c r="G52" s="4">
-        <v>5</v>
+      <c r="G52" s="31">
+        <v>6</v>
       </c>
       <c r="H52" s="4">
         <v>0</v>
@@ -4449,8 +4452,8 @@
       <c r="F53" s="4">
         <v>1</v>
       </c>
-      <c r="G53" s="4">
-        <v>3</v>
+      <c r="G53" s="31">
+        <v>4</v>
       </c>
       <c r="H53" s="4">
         <v>0</v>
@@ -4488,7 +4491,7 @@
       <c r="F54" s="4">
         <v>0</v>
       </c>
-      <c r="G54" s="4">
+      <c r="G54" s="31">
         <v>6</v>
       </c>
       <c r="H54" s="4">
@@ -4527,7 +4530,7 @@
       <c r="F55" s="4">
         <v>0</v>
       </c>
-      <c r="G55" s="4">
+      <c r="G55" s="31">
         <v>4</v>
       </c>
       <c r="H55" s="4">
@@ -4566,7 +4569,7 @@
       <c r="F56" s="4">
         <v>0</v>
       </c>
-      <c r="G56" s="4">
+      <c r="G56" s="31">
         <v>2</v>
       </c>
       <c r="H56" s="4">
@@ -4605,7 +4608,7 @@
       <c r="F57" s="4">
         <v>1</v>
       </c>
-      <c r="G57" s="4">
+      <c r="G57" s="31">
         <v>3</v>
       </c>
       <c r="H57" s="4">
@@ -4644,7 +4647,7 @@
       <c r="F58" s="4">
         <v>0</v>
       </c>
-      <c r="G58" s="4">
+      <c r="G58" s="31">
         <v>6</v>
       </c>
       <c r="H58" s="4">
@@ -4683,7 +4686,7 @@
       <c r="F59" s="4">
         <v>0</v>
       </c>
-      <c r="G59" s="4">
+      <c r="G59" s="31">
         <v>2</v>
       </c>
       <c r="H59" s="4">
@@ -4722,8 +4725,8 @@
       <c r="F60" s="4">
         <v>1</v>
       </c>
-      <c r="G60" s="4">
-        <v>6</v>
+      <c r="G60" s="31">
+        <v>7</v>
       </c>
       <c r="H60" s="4">
         <v>0</v>
@@ -4761,8 +4764,8 @@
       <c r="F61" s="4">
         <v>5</v>
       </c>
-      <c r="G61" s="4">
-        <v>0</v>
+      <c r="G61" s="31">
+        <v>1</v>
       </c>
       <c r="H61" s="4">
         <v>0</v>
@@ -4800,7 +4803,7 @@
       <c r="F62" s="4">
         <v>6</v>
       </c>
-      <c r="G62" s="4">
+      <c r="G62" s="31">
         <v>6</v>
       </c>
       <c r="H62" s="4">
@@ -4839,8 +4842,8 @@
       <c r="F63" s="4">
         <v>7</v>
       </c>
-      <c r="G63" s="4">
-        <v>4</v>
+      <c r="G63" s="31">
+        <v>5</v>
       </c>
       <c r="H63" s="4">
         <v>0</v>
@@ -4878,7 +4881,7 @@
       <c r="F64" s="4">
         <v>6</v>
       </c>
-      <c r="G64" s="4">
+      <c r="G64" s="31">
         <v>4</v>
       </c>
       <c r="H64" s="4">
@@ -4917,8 +4920,8 @@
       <c r="F65" s="4">
         <v>6</v>
       </c>
-      <c r="G65" s="4">
-        <v>0</v>
+      <c r="G65" s="31">
+        <v>1</v>
       </c>
       <c r="H65" s="4">
         <v>0</v>
@@ -4956,7 +4959,7 @@
       <c r="F66" s="4">
         <v>7</v>
       </c>
-      <c r="G66" s="4">
+      <c r="G66" s="31">
         <v>3</v>
       </c>
       <c r="H66" s="4">
@@ -5002,7 +5005,7 @@
       </c>
       <c r="G67" s="6">
         <f t="shared" si="0"/>
-        <v>249</v>
+        <v>279</v>
       </c>
       <c r="H67" s="6">
         <f t="shared" si="0"/>
@@ -5032,7 +5035,7 @@
       </c>
       <c r="F68">
         <f>G67</f>
-        <v>249</v>
+        <v>279</v>
       </c>
       <c r="J68">
         <f>B67-C67</f>
@@ -5087,7 +5090,7 @@
     <row r="73" spans="1:13" x14ac:dyDescent="0.25">
       <c r="F73">
         <f>SUM(F68:F72)</f>
-        <v>755</v>
+        <v>785</v>
       </c>
       <c r="J73" s="3" t="s">
         <v>17</v>
@@ -5096,7 +5099,7 @@
     <row r="74" spans="1:13" x14ac:dyDescent="0.25">
       <c r="F74">
         <f>K67-F73</f>
-        <v>2523</v>
+        <v>2493</v>
       </c>
       <c r="J74">
         <f>J72-L67</f>
@@ -8047,7 +8050,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L68"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A53" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" sqref="A1:L58"/>
     </sheetView>

</xml_diff>

<commit_message>
nmv 29 05 2022
</commit_message>
<xml_diff>
--- a/TS Jatai Ghanam Project/Stas table for TS 2.1 TO 2.6.xlsx
+++ b/TS Jatai Ghanam Project/Stas table for TS 2.1 TO 2.6.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7095"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7095" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="TS 2.1" sheetId="8" r:id="rId1"/>
@@ -2018,7 +2018,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
@@ -2103,6 +2103,9 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -2387,7 +2390,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M77"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A62" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="R62" sqref="R62"/>
     </sheetView>
@@ -5133,9 +5136,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L83"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A71" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E74" sqref="E74:J83"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A65" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" sqref="A1:L73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5143,7 +5146,7 @@
     <col min="1" max="1" width="12.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="5.85546875" customWidth="1"/>
     <col min="3" max="3" width="7.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="4.42578125" customWidth="1"/>
+    <col min="4" max="4" width="5.5703125" customWidth="1"/>
     <col min="5" max="5" width="7.42578125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="6.5703125" customWidth="1"/>
     <col min="8" max="8" width="8.85546875" bestFit="1" customWidth="1"/>
@@ -5209,7 +5212,7 @@
       <c r="F2" s="25">
         <v>0</v>
       </c>
-      <c r="G2" s="25">
+      <c r="G2" s="32">
         <v>6</v>
       </c>
       <c r="H2" s="25">
@@ -5247,7 +5250,7 @@
       <c r="F3" s="25">
         <v>0</v>
       </c>
-      <c r="G3" s="25">
+      <c r="G3" s="32">
         <v>7</v>
       </c>
       <c r="H3" s="25">
@@ -5285,8 +5288,8 @@
       <c r="F4" s="25">
         <v>0</v>
       </c>
-      <c r="G4" s="25">
-        <v>5</v>
+      <c r="G4" s="32">
+        <v>6</v>
       </c>
       <c r="H4" s="25">
         <v>0</v>
@@ -5323,7 +5326,7 @@
       <c r="F5" s="25">
         <v>0</v>
       </c>
-      <c r="G5" s="25">
+      <c r="G5" s="32">
         <v>6</v>
       </c>
       <c r="H5" s="25">
@@ -5361,8 +5364,8 @@
       <c r="F6" s="25">
         <v>1</v>
       </c>
-      <c r="G6" s="25">
-        <v>4</v>
+      <c r="G6" s="32">
+        <v>6</v>
       </c>
       <c r="H6" s="25">
         <v>0</v>
@@ -5399,7 +5402,7 @@
       <c r="F7" s="25">
         <v>0</v>
       </c>
-      <c r="G7" s="25">
+      <c r="G7" s="32">
         <v>4</v>
       </c>
       <c r="H7" s="25">
@@ -5437,7 +5440,7 @@
       <c r="F8" s="25">
         <v>0</v>
       </c>
-      <c r="G8" s="25">
+      <c r="G8" s="32">
         <v>7</v>
       </c>
       <c r="H8" s="25">
@@ -5475,7 +5478,7 @@
       <c r="F9" s="25">
         <v>0</v>
       </c>
-      <c r="G9" s="25">
+      <c r="G9" s="32">
         <v>4</v>
       </c>
       <c r="H9" s="25">
@@ -5513,8 +5516,8 @@
       <c r="F10" s="25">
         <v>0</v>
       </c>
-      <c r="G10" s="25">
-        <v>3</v>
+      <c r="G10" s="32">
+        <v>4</v>
       </c>
       <c r="H10" s="25">
         <v>0</v>
@@ -5551,7 +5554,7 @@
       <c r="F11" s="25">
         <v>1</v>
       </c>
-      <c r="G11" s="25">
+      <c r="G11" s="32">
         <v>5</v>
       </c>
       <c r="H11" s="25">
@@ -5589,7 +5592,7 @@
       <c r="F12" s="25">
         <v>0</v>
       </c>
-      <c r="G12" s="25">
+      <c r="G12" s="32">
         <v>6</v>
       </c>
       <c r="H12" s="25">
@@ -5627,7 +5630,7 @@
       <c r="F13" s="25">
         <v>0</v>
       </c>
-      <c r="G13" s="25">
+      <c r="G13" s="32">
         <v>5</v>
       </c>
       <c r="H13" s="25">
@@ -5665,7 +5668,7 @@
       <c r="F14" s="25">
         <v>0</v>
       </c>
-      <c r="G14" s="25">
+      <c r="G14" s="32">
         <v>4</v>
       </c>
       <c r="H14" s="25">
@@ -5703,7 +5706,7 @@
       <c r="F15" s="25">
         <v>1</v>
       </c>
-      <c r="G15" s="25">
+      <c r="G15" s="32">
         <v>4</v>
       </c>
       <c r="H15" s="25">
@@ -5741,7 +5744,7 @@
       <c r="F16" s="25">
         <v>0</v>
       </c>
-      <c r="G16" s="25">
+      <c r="G16" s="32">
         <v>4</v>
       </c>
       <c r="H16" s="25">
@@ -5779,7 +5782,7 @@
       <c r="F17" s="25">
         <v>0</v>
       </c>
-      <c r="G17" s="25">
+      <c r="G17" s="32">
         <v>3</v>
       </c>
       <c r="H17" s="25">
@@ -5817,7 +5820,7 @@
       <c r="F18" s="25">
         <v>0</v>
       </c>
-      <c r="G18" s="25">
+      <c r="G18" s="32">
         <v>1</v>
       </c>
       <c r="H18" s="25">
@@ -5855,7 +5858,7 @@
       <c r="F19" s="25">
         <v>0</v>
       </c>
-      <c r="G19" s="25">
+      <c r="G19" s="32">
         <v>5</v>
       </c>
       <c r="H19" s="25">
@@ -5893,7 +5896,7 @@
       <c r="F20" s="25">
         <v>0</v>
       </c>
-      <c r="G20" s="25">
+      <c r="G20" s="32">
         <v>4</v>
       </c>
       <c r="H20" s="25">
@@ -5931,7 +5934,7 @@
       <c r="F21" s="25">
         <v>0</v>
       </c>
-      <c r="G21" s="25">
+      <c r="G21" s="32">
         <v>2</v>
       </c>
       <c r="H21" s="25">
@@ -5969,8 +5972,8 @@
       <c r="F22" s="25">
         <v>0</v>
       </c>
-      <c r="G22" s="25">
-        <v>5</v>
+      <c r="G22" s="32">
+        <v>7</v>
       </c>
       <c r="H22" s="25">
         <v>0</v>
@@ -6007,7 +6010,7 @@
       <c r="F23" s="25">
         <v>2</v>
       </c>
-      <c r="G23" s="25">
+      <c r="G23" s="32">
         <v>3</v>
       </c>
       <c r="H23" s="25">
@@ -6045,7 +6048,7 @@
       <c r="F24" s="25">
         <v>0</v>
       </c>
-      <c r="G24" s="25">
+      <c r="G24" s="32">
         <v>3</v>
       </c>
       <c r="H24" s="25">
@@ -6083,7 +6086,7 @@
       <c r="F25" s="25">
         <v>0</v>
       </c>
-      <c r="G25" s="25">
+      <c r="G25" s="32">
         <v>2</v>
       </c>
       <c r="H25" s="25">
@@ -6121,7 +6124,7 @@
       <c r="F26" s="25">
         <v>0</v>
       </c>
-      <c r="G26" s="25">
+      <c r="G26" s="32">
         <v>1</v>
       </c>
       <c r="H26" s="25">
@@ -6159,7 +6162,7 @@
       <c r="F27" s="25">
         <v>0</v>
       </c>
-      <c r="G27" s="25">
+      <c r="G27" s="32">
         <v>3</v>
       </c>
       <c r="H27" s="25">
@@ -6197,7 +6200,7 @@
       <c r="F28" s="25">
         <v>0</v>
       </c>
-      <c r="G28" s="25">
+      <c r="G28" s="32">
         <v>1</v>
       </c>
       <c r="H28" s="25">
@@ -6235,7 +6238,7 @@
       <c r="F29" s="25">
         <v>0</v>
       </c>
-      <c r="G29" s="25">
+      <c r="G29" s="32">
         <v>2</v>
       </c>
       <c r="H29" s="25">
@@ -6273,7 +6276,7 @@
       <c r="F30" s="25">
         <v>1</v>
       </c>
-      <c r="G30" s="25">
+      <c r="G30" s="32">
         <v>3</v>
       </c>
       <c r="H30" s="25">
@@ -6311,7 +6314,7 @@
       <c r="F31" s="25">
         <v>0</v>
       </c>
-      <c r="G31" s="25">
+      <c r="G31" s="32">
         <v>3</v>
       </c>
       <c r="H31" s="25">
@@ -6349,7 +6352,7 @@
       <c r="F32" s="25">
         <v>0</v>
       </c>
-      <c r="G32" s="25">
+      <c r="G32" s="32">
         <v>3</v>
       </c>
       <c r="H32" s="25">
@@ -6387,8 +6390,8 @@
       <c r="F33" s="25">
         <v>0</v>
       </c>
-      <c r="G33" s="25">
-        <v>3</v>
+      <c r="G33" s="32">
+        <v>6</v>
       </c>
       <c r="H33" s="25">
         <v>0</v>
@@ -6425,8 +6428,8 @@
       <c r="F34" s="25">
         <v>0</v>
       </c>
-      <c r="G34" s="25">
-        <v>2</v>
+      <c r="G34" s="32">
+        <v>4</v>
       </c>
       <c r="H34" s="25">
         <v>0</v>
@@ -6463,7 +6466,7 @@
       <c r="F35" s="25">
         <v>1</v>
       </c>
-      <c r="G35" s="25">
+      <c r="G35" s="32">
         <v>4</v>
       </c>
       <c r="H35" s="25">
@@ -6501,7 +6504,7 @@
       <c r="F36" s="25">
         <v>0</v>
       </c>
-      <c r="G36" s="25">
+      <c r="G36" s="32">
         <v>6</v>
       </c>
       <c r="H36" s="25">
@@ -6539,7 +6542,7 @@
       <c r="F37" s="25">
         <v>0</v>
       </c>
-      <c r="G37" s="25">
+      <c r="G37" s="32">
         <v>4</v>
       </c>
       <c r="H37" s="25">
@@ -6577,8 +6580,8 @@
       <c r="F38" s="25">
         <v>0</v>
       </c>
-      <c r="G38" s="25">
-        <v>3</v>
+      <c r="G38" s="32">
+        <v>4</v>
       </c>
       <c r="H38" s="25">
         <v>0</v>
@@ -6615,7 +6618,7 @@
       <c r="F39" s="25">
         <v>0</v>
       </c>
-      <c r="G39" s="25">
+      <c r="G39" s="32">
         <v>6</v>
       </c>
       <c r="H39" s="25">
@@ -6653,7 +6656,7 @@
       <c r="F40" s="25">
         <v>1</v>
       </c>
-      <c r="G40" s="25">
+      <c r="G40" s="32">
         <v>6</v>
       </c>
       <c r="H40" s="25">
@@ -6691,7 +6694,7 @@
       <c r="F41" s="25">
         <v>0</v>
       </c>
-      <c r="G41" s="25">
+      <c r="G41" s="32">
         <v>6</v>
       </c>
       <c r="H41" s="25">
@@ -6729,7 +6732,7 @@
       <c r="F42" s="25">
         <v>0</v>
       </c>
-      <c r="G42" s="25">
+      <c r="G42" s="32">
         <v>4</v>
       </c>
       <c r="H42" s="25">
@@ -6767,7 +6770,7 @@
       <c r="F43" s="25">
         <v>0</v>
       </c>
-      <c r="G43" s="25">
+      <c r="G43" s="32">
         <v>3</v>
       </c>
       <c r="H43" s="25">
@@ -6805,7 +6808,7 @@
       <c r="F44" s="25">
         <v>0</v>
       </c>
-      <c r="G44" s="25">
+      <c r="G44" s="32">
         <v>5</v>
       </c>
       <c r="H44" s="25">
@@ -6843,7 +6846,7 @@
       <c r="F45" s="25">
         <v>0</v>
       </c>
-      <c r="G45" s="25">
+      <c r="G45" s="32">
         <v>3</v>
       </c>
       <c r="H45" s="25">
@@ -6881,7 +6884,7 @@
       <c r="F46" s="25">
         <v>1</v>
       </c>
-      <c r="G46" s="25">
+      <c r="G46" s="32">
         <v>6</v>
       </c>
       <c r="H46" s="25">
@@ -6919,7 +6922,7 @@
       <c r="F47" s="25">
         <v>0</v>
       </c>
-      <c r="G47" s="25">
+      <c r="G47" s="32">
         <v>4</v>
       </c>
       <c r="H47" s="25">
@@ -6957,8 +6960,8 @@
       <c r="F48" s="25">
         <v>0</v>
       </c>
-      <c r="G48" s="25">
-        <v>2</v>
+      <c r="G48" s="32">
+        <v>4</v>
       </c>
       <c r="H48" s="25">
         <v>0</v>
@@ -6995,7 +6998,7 @@
       <c r="F49" s="25">
         <v>0</v>
       </c>
-      <c r="G49" s="25">
+      <c r="G49" s="32">
         <v>6</v>
       </c>
       <c r="H49" s="25">
@@ -7033,8 +7036,8 @@
       <c r="F50" s="25">
         <v>0</v>
       </c>
-      <c r="G50" s="25">
-        <v>3</v>
+      <c r="G50" s="32">
+        <v>4</v>
       </c>
       <c r="H50" s="25">
         <v>0</v>
@@ -7071,8 +7074,8 @@
       <c r="F51" s="25">
         <v>0</v>
       </c>
-      <c r="G51" s="25">
-        <v>3</v>
+      <c r="G51" s="32">
+        <v>4</v>
       </c>
       <c r="H51" s="25">
         <v>0</v>
@@ -7109,7 +7112,7 @@
       <c r="F52" s="25">
         <v>0</v>
       </c>
-      <c r="G52" s="25">
+      <c r="G52" s="32">
         <v>2</v>
       </c>
       <c r="H52" s="25">
@@ -7147,7 +7150,7 @@
       <c r="F53" s="25">
         <v>1</v>
       </c>
-      <c r="G53" s="25">
+      <c r="G53" s="32">
         <v>1</v>
       </c>
       <c r="H53" s="25">
@@ -7185,7 +7188,7 @@
       <c r="F54" s="25">
         <v>0</v>
       </c>
-      <c r="G54" s="25">
+      <c r="G54" s="32">
         <v>5</v>
       </c>
       <c r="H54" s="25">
@@ -7223,8 +7226,8 @@
       <c r="F55" s="25">
         <v>0</v>
       </c>
-      <c r="G55" s="25">
-        <v>1</v>
+      <c r="G55" s="32">
+        <v>2</v>
       </c>
       <c r="H55" s="25">
         <v>0</v>
@@ -7261,7 +7264,7 @@
       <c r="F56" s="25">
         <v>0</v>
       </c>
-      <c r="G56" s="25">
+      <c r="G56" s="32">
         <v>3</v>
       </c>
       <c r="H56" s="25">
@@ -7299,7 +7302,7 @@
       <c r="F57" s="25">
         <v>0</v>
       </c>
-      <c r="G57" s="25">
+      <c r="G57" s="32">
         <v>4</v>
       </c>
       <c r="H57" s="25">
@@ -7337,7 +7340,7 @@
       <c r="F58" s="25">
         <v>1</v>
       </c>
-      <c r="G58" s="25">
+      <c r="G58" s="32">
         <v>2</v>
       </c>
       <c r="H58" s="25">
@@ -7375,7 +7378,7 @@
       <c r="F59" s="25">
         <v>0</v>
       </c>
-      <c r="G59" s="25">
+      <c r="G59" s="32">
         <v>6</v>
       </c>
       <c r="H59" s="25">
@@ -7413,7 +7416,7 @@
       <c r="F60" s="25">
         <v>0</v>
       </c>
-      <c r="G60" s="25">
+      <c r="G60" s="32">
         <v>3</v>
       </c>
       <c r="H60" s="25">
@@ -7451,7 +7454,7 @@
       <c r="F61" s="25">
         <v>0</v>
       </c>
-      <c r="G61" s="25">
+      <c r="G61" s="32">
         <v>5</v>
       </c>
       <c r="H61" s="25">
@@ -7489,7 +7492,7 @@
       <c r="F62" s="25">
         <v>0</v>
       </c>
-      <c r="G62" s="25">
+      <c r="G62" s="32">
         <v>4</v>
       </c>
       <c r="H62" s="25">
@@ -7527,7 +7530,7 @@
       <c r="F63" s="25">
         <v>0</v>
       </c>
-      <c r="G63" s="25">
+      <c r="G63" s="32">
         <v>4</v>
       </c>
       <c r="H63" s="25">
@@ -7565,8 +7568,8 @@
       <c r="F64" s="25">
         <v>1</v>
       </c>
-      <c r="G64" s="25">
-        <v>4</v>
+      <c r="G64" s="32">
+        <v>6</v>
       </c>
       <c r="H64" s="25">
         <v>0</v>
@@ -7603,7 +7606,7 @@
       <c r="F65" s="25">
         <v>6</v>
       </c>
-      <c r="G65" s="25">
+      <c r="G65" s="32">
         <v>3</v>
       </c>
       <c r="H65" s="25">
@@ -7641,7 +7644,7 @@
       <c r="F66" s="25">
         <v>7</v>
       </c>
-      <c r="G66" s="25">
+      <c r="G66" s="32">
         <v>2</v>
       </c>
       <c r="H66" s="25">
@@ -7679,7 +7682,7 @@
       <c r="F67" s="25">
         <v>7</v>
       </c>
-      <c r="G67" s="25">
+      <c r="G67" s="32">
         <v>3</v>
       </c>
       <c r="H67" s="25">
@@ -7717,7 +7720,7 @@
       <c r="F68" s="25">
         <v>5</v>
       </c>
-      <c r="G68" s="25">
+      <c r="G68" s="32">
         <v>1</v>
       </c>
       <c r="H68" s="25">
@@ -7755,7 +7758,7 @@
       <c r="F69" s="25">
         <v>5</v>
       </c>
-      <c r="G69" s="25">
+      <c r="G69" s="32">
         <v>3</v>
       </c>
       <c r="H69" s="25">
@@ -7793,7 +7796,7 @@
       <c r="F70" s="25">
         <v>6</v>
       </c>
-      <c r="G70" s="25">
+      <c r="G70" s="32">
         <v>3</v>
       </c>
       <c r="H70" s="25">
@@ -7831,7 +7834,7 @@
       <c r="F71" s="25">
         <v>7</v>
       </c>
-      <c r="G71" s="25">
+      <c r="G71" s="32">
         <v>5</v>
       </c>
       <c r="H71" s="25">
@@ -7869,7 +7872,7 @@
       <c r="F72" s="25">
         <v>6</v>
       </c>
-      <c r="G72" s="25">
+      <c r="G72" s="32">
         <v>3</v>
       </c>
       <c r="H72" s="25">
@@ -7914,7 +7917,7 @@
       </c>
       <c r="G73" s="28">
         <f t="shared" si="0"/>
-        <v>264</v>
+        <v>283</v>
       </c>
       <c r="H73" s="28">
         <f t="shared" si="0"/>
@@ -7946,7 +7949,7 @@
       </c>
       <c r="F74">
         <f>G73</f>
-        <v>264</v>
+        <v>283</v>
       </c>
       <c r="J74">
         <f>B73-C73</f>
@@ -8007,7 +8010,7 @@
     <row r="79" spans="1:12" x14ac:dyDescent="0.25">
       <c r="F79">
         <f>SUM(F74:F78)</f>
-        <v>983</v>
+        <v>1002</v>
       </c>
       <c r="J79" s="3" t="s">
         <v>17</v>
@@ -8016,7 +8019,7 @@
     <row r="80" spans="1:12" x14ac:dyDescent="0.25">
       <c r="F80">
         <f>K73-F79</f>
-        <v>2543</v>
+        <v>2524</v>
       </c>
       <c r="J80">
         <f>J78-L73</f>

</xml_diff>

<commit_message>
nmv 31 05 2022
</commit_message>
<xml_diff>
--- a/TS Jatai Ghanam Project/Stas table for TS 2.1 TO 2.6.xlsx
+++ b/TS Jatai Ghanam Project/Stas table for TS 2.1 TO 2.6.xlsx
@@ -10536,11 +10536,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="F51" sqref="F51:F54"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="A50" sqref="A50:L50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="5.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="3.85546875" customWidth="1"/>
+    <col min="5" max="5" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="5.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="3.42578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="7.42578125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="89.25" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
@@ -12409,47 +12420,47 @@
         <v>48</v>
       </c>
       <c r="B50" s="30">
-        <f>SUM(B2:B49)</f>
+        <f t="shared" ref="B50:L50" si="0">SUM(B2:B49)</f>
         <v>295</v>
       </c>
       <c r="C50" s="30">
-        <f>SUM(C2:C49)</f>
+        <f t="shared" si="0"/>
         <v>13</v>
       </c>
       <c r="D50" s="30">
-        <f>SUM(D2:D49)</f>
+        <f t="shared" si="0"/>
         <v>9</v>
       </c>
       <c r="E50" s="30">
-        <f>SUM(E2:E49)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="F50" s="30">
-        <f>SUM(F2:F49)</f>
+        <f t="shared" si="0"/>
         <v>72</v>
       </c>
       <c r="G50" s="30">
-        <f>SUM(G2:G49)</f>
+        <f t="shared" si="0"/>
         <v>178</v>
       </c>
       <c r="H50" s="30">
-        <f>SUM(H2:H49)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="I50" s="30">
-        <f>SUM(I2:I49)</f>
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
       <c r="J50" s="30">
-        <f>SUM(J2:J49)</f>
+        <f t="shared" si="0"/>
         <v>2044</v>
       </c>
       <c r="K50" s="30">
-        <f>SUM(K2:K49)</f>
+        <f t="shared" si="0"/>
         <v>2406</v>
       </c>
       <c r="L50" s="30">
-        <f>SUM(L2:L49)</f>
+        <f t="shared" si="0"/>
         <v>2696</v>
       </c>
     </row>

</xml_diff>

<commit_message>
nmv 23 07 2022
</commit_message>
<xml_diff>
--- a/TS Jatai Ghanam Project/Stas table for TS 2.1 TO 2.6.xlsx
+++ b/TS Jatai Ghanam Project/Stas table for TS 2.1 TO 2.6.xlsx
@@ -9,14 +9,15 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7095" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7095" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="TS 2.1" sheetId="8" r:id="rId1"/>
     <sheet name="TS 2.2" sheetId="9" r:id="rId2"/>
     <sheet name="TS 2.3" sheetId="10" r:id="rId3"/>
     <sheet name="TS 2.4" sheetId="11" r:id="rId4"/>
-    <sheet name="total 2.1 to 2.6" sheetId="7" r:id="rId5"/>
+    <sheet name="TS 2.5" sheetId="12" r:id="rId5"/>
+    <sheet name="total 2.1 to 2.6" sheetId="7" r:id="rId6"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="355" uniqueCount="285">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="449" uniqueCount="359">
   <si>
     <t>Panchaati Ref</t>
   </si>
@@ -1990,12 +1991,234 @@
   <si>
     <t>2.4.14.5</t>
   </si>
+  <si>
+    <t>2.5.1.1 :</t>
+  </si>
+  <si>
+    <t>2.5.1.2 :</t>
+  </si>
+  <si>
+    <t>2.5.1.3 :</t>
+  </si>
+  <si>
+    <t>2.5.1.4 :</t>
+  </si>
+  <si>
+    <t>2.5.1.5 :</t>
+  </si>
+  <si>
+    <t>2.5.1.6 :</t>
+  </si>
+  <si>
+    <t>2.5.1.7 :</t>
+  </si>
+  <si>
+    <t>2.5.2.1 :</t>
+  </si>
+  <si>
+    <t>2.5.2.2 :</t>
+  </si>
+  <si>
+    <t>2.5.2.3 :</t>
+  </si>
+  <si>
+    <t>2.5.2.4 :</t>
+  </si>
+  <si>
+    <t>2.5.2.5 :</t>
+  </si>
+  <si>
+    <t>2.5.2.6 :</t>
+  </si>
+  <si>
+    <t>2.5.2.7 :</t>
+  </si>
+  <si>
+    <t>2.5.3.1 :</t>
+  </si>
+  <si>
+    <t>2.5.3.2 :</t>
+  </si>
+  <si>
+    <t>2.5.3.3 :</t>
+  </si>
+  <si>
+    <t>2.5.3.4 :</t>
+  </si>
+  <si>
+    <t>2.5.3.5 :</t>
+  </si>
+  <si>
+    <t>2.5.3.6 :</t>
+  </si>
+  <si>
+    <t>2.5.3.7 :</t>
+  </si>
+  <si>
+    <t>2.5.4.1 :</t>
+  </si>
+  <si>
+    <t>2.5.4.2 :</t>
+  </si>
+  <si>
+    <t>2.5.4.3 :</t>
+  </si>
+  <si>
+    <t>2.5.4.4 :</t>
+  </si>
+  <si>
+    <t>2.5.4.5 :</t>
+  </si>
+  <si>
+    <t>2.5.5.1 :</t>
+  </si>
+  <si>
+    <t>2.5.5.2 :</t>
+  </si>
+  <si>
+    <t>2.5.5.3 :</t>
+  </si>
+  <si>
+    <t>2.5.5.4 :</t>
+  </si>
+  <si>
+    <t>2.5.5.5 :</t>
+  </si>
+  <si>
+    <t>2.5.5.6 :</t>
+  </si>
+  <si>
+    <t>2.5.6.1 :</t>
+  </si>
+  <si>
+    <t>2.5.6.2 :</t>
+  </si>
+  <si>
+    <t>2.5.6.3 :</t>
+  </si>
+  <si>
+    <t>2.5.6.4 :</t>
+  </si>
+  <si>
+    <t>2.5.6.5 :</t>
+  </si>
+  <si>
+    <t>2.5.6.6 :</t>
+  </si>
+  <si>
+    <t>2.5.7.1 :</t>
+  </si>
+  <si>
+    <t>2.5.7.2 :</t>
+  </si>
+  <si>
+    <t>2.5.7.3 :</t>
+  </si>
+  <si>
+    <t>2.5.7.4 :</t>
+  </si>
+  <si>
+    <t>2.5.7.5 :</t>
+  </si>
+  <si>
+    <t>2.5.8.1 :</t>
+  </si>
+  <si>
+    <t>2.5.8.2 :</t>
+  </si>
+  <si>
+    <t>2.5.8.3 :</t>
+  </si>
+  <si>
+    <t>2.5.8.4 :</t>
+  </si>
+  <si>
+    <t>2.5.8.5 :</t>
+  </si>
+  <si>
+    <t>2.5.8.6 :</t>
+  </si>
+  <si>
+    <t>2.5.8.7 :</t>
+  </si>
+  <si>
+    <t>2.5.9.1 :</t>
+  </si>
+  <si>
+    <t>2.5.9.2 :</t>
+  </si>
+  <si>
+    <t>2.5.9.3 :</t>
+  </si>
+  <si>
+    <t>2.5.9.4 :</t>
+  </si>
+  <si>
+    <t>2.5.9.5 :</t>
+  </si>
+  <si>
+    <t>2.5.9.6 :</t>
+  </si>
+  <si>
+    <t>2.5.10.1 :</t>
+  </si>
+  <si>
+    <t>2.5.10.2 :</t>
+  </si>
+  <si>
+    <t>2.5.10.3 :</t>
+  </si>
+  <si>
+    <t>2.5.10.4 :</t>
+  </si>
+  <si>
+    <t>2.5.11.1 :</t>
+  </si>
+  <si>
+    <t>2.5.11.2 :</t>
+  </si>
+  <si>
+    <t>2.5.11.3 :</t>
+  </si>
+  <si>
+    <t>2.5.11.4 :</t>
+  </si>
+  <si>
+    <t>2.5.11.5 :</t>
+  </si>
+  <si>
+    <t>2.5.11.6 :</t>
+  </si>
+  <si>
+    <t>2.5.11.7 :</t>
+  </si>
+  <si>
+    <t>2.5.11.8 :</t>
+  </si>
+  <si>
+    <t>2.5.11.9 :</t>
+  </si>
+  <si>
+    <t>2.5.12.1 :</t>
+  </si>
+  <si>
+    <t>2.5.12.2 :</t>
+  </si>
+  <si>
+    <t>2.5.12.3 :</t>
+  </si>
+  <si>
+    <t>2.5.12.4 :</t>
+  </si>
+  <si>
+    <t>2.5.12.5 :</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2076,6 +2299,12 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -2163,7 +2392,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
@@ -2253,6 +2482,14 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -10536,8 +10773,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="A50" sqref="A50:L50"/>
+    <sheetView topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="E50" sqref="E50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12565,9 +12802,3032 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:L86"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A67" workbookViewId="0">
+      <selection sqref="A1:L76"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11" customWidth="1"/>
+    <col min="2" max="2" width="6.7109375" customWidth="1"/>
+    <col min="3" max="3" width="7.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="4.42578125" customWidth="1"/>
+    <col min="5" max="5" width="7.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="5.7109375" customWidth="1"/>
+    <col min="8" max="8" width="9" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="6.28515625" customWidth="1"/>
+    <col min="10" max="10" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="7.5703125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" ht="89.25" x14ac:dyDescent="0.25">
+      <c r="A1" s="33" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="33" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="33" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="33" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="33" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="33" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="33" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="33" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="33" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="33" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="33" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="33" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2" s="34" t="s">
+        <v>285</v>
+      </c>
+      <c r="B2" s="34">
+        <v>12</v>
+      </c>
+      <c r="C2" s="34">
+        <v>0</v>
+      </c>
+      <c r="D2" s="34">
+        <v>0</v>
+      </c>
+      <c r="E2" s="34">
+        <v>0</v>
+      </c>
+      <c r="F2" s="34">
+        <v>0</v>
+      </c>
+      <c r="G2" s="34">
+        <v>1</v>
+      </c>
+      <c r="H2" s="34">
+        <v>0</v>
+      </c>
+      <c r="I2" s="34">
+        <v>0</v>
+      </c>
+      <c r="J2" s="34">
+        <v>38</v>
+      </c>
+      <c r="K2" s="34">
+        <v>50</v>
+      </c>
+      <c r="L2" s="34">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A3" s="34" t="s">
+        <v>286</v>
+      </c>
+      <c r="B3" s="34">
+        <v>7</v>
+      </c>
+      <c r="C3" s="34">
+        <v>0</v>
+      </c>
+      <c r="D3" s="34">
+        <v>0</v>
+      </c>
+      <c r="E3" s="34">
+        <v>0</v>
+      </c>
+      <c r="F3" s="34">
+        <v>0</v>
+      </c>
+      <c r="G3" s="34">
+        <v>5</v>
+      </c>
+      <c r="H3" s="34">
+        <v>0</v>
+      </c>
+      <c r="I3" s="34">
+        <v>0</v>
+      </c>
+      <c r="J3" s="34">
+        <v>43</v>
+      </c>
+      <c r="K3" s="34">
+        <v>50</v>
+      </c>
+      <c r="L3" s="34">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A4" s="34" t="s">
+        <v>287</v>
+      </c>
+      <c r="B4" s="34">
+        <v>10</v>
+      </c>
+      <c r="C4" s="34">
+        <v>0</v>
+      </c>
+      <c r="D4" s="34">
+        <v>0</v>
+      </c>
+      <c r="E4" s="34">
+        <v>0</v>
+      </c>
+      <c r="F4" s="34">
+        <v>0</v>
+      </c>
+      <c r="G4" s="34">
+        <v>6</v>
+      </c>
+      <c r="H4" s="34">
+        <v>0</v>
+      </c>
+      <c r="I4" s="34">
+        <v>0</v>
+      </c>
+      <c r="J4" s="34">
+        <v>40</v>
+      </c>
+      <c r="K4" s="34">
+        <v>50</v>
+      </c>
+      <c r="L4" s="34">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A5" s="34" t="s">
+        <v>288</v>
+      </c>
+      <c r="B5" s="34">
+        <v>10</v>
+      </c>
+      <c r="C5" s="34">
+        <v>0</v>
+      </c>
+      <c r="D5" s="34">
+        <v>1</v>
+      </c>
+      <c r="E5" s="34">
+        <v>0</v>
+      </c>
+      <c r="F5" s="34">
+        <v>0</v>
+      </c>
+      <c r="G5" s="34">
+        <v>4</v>
+      </c>
+      <c r="H5" s="34">
+        <v>0</v>
+      </c>
+      <c r="I5" s="34">
+        <v>0</v>
+      </c>
+      <c r="J5" s="34">
+        <v>39</v>
+      </c>
+      <c r="K5" s="34">
+        <v>50</v>
+      </c>
+      <c r="L5" s="34">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A6" s="34" t="s">
+        <v>289</v>
+      </c>
+      <c r="B6" s="34">
+        <v>10</v>
+      </c>
+      <c r="C6" s="34">
+        <v>0</v>
+      </c>
+      <c r="D6" s="34">
+        <v>0</v>
+      </c>
+      <c r="E6" s="34">
+        <v>0</v>
+      </c>
+      <c r="F6" s="34">
+        <v>0</v>
+      </c>
+      <c r="G6" s="34">
+        <v>8</v>
+      </c>
+      <c r="H6" s="34">
+        <v>0</v>
+      </c>
+      <c r="I6" s="34">
+        <v>0</v>
+      </c>
+      <c r="J6" s="34">
+        <v>40</v>
+      </c>
+      <c r="K6" s="34">
+        <v>50</v>
+      </c>
+      <c r="L6" s="34">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A7" s="34" t="s">
+        <v>290</v>
+      </c>
+      <c r="B7" s="34">
+        <v>11</v>
+      </c>
+      <c r="C7" s="34">
+        <v>0</v>
+      </c>
+      <c r="D7" s="34">
+        <v>1</v>
+      </c>
+      <c r="E7" s="34">
+        <v>0</v>
+      </c>
+      <c r="F7" s="34">
+        <v>0</v>
+      </c>
+      <c r="G7" s="34">
+        <v>0</v>
+      </c>
+      <c r="H7" s="34">
+        <v>0</v>
+      </c>
+      <c r="I7" s="34">
+        <v>0</v>
+      </c>
+      <c r="J7" s="34">
+        <v>38</v>
+      </c>
+      <c r="K7" s="34">
+        <v>50</v>
+      </c>
+      <c r="L7" s="34">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A8" s="34" t="s">
+        <v>291</v>
+      </c>
+      <c r="B8" s="34">
+        <v>10</v>
+      </c>
+      <c r="C8" s="34">
+        <v>0</v>
+      </c>
+      <c r="D8" s="34">
+        <v>0</v>
+      </c>
+      <c r="E8" s="34">
+        <v>0</v>
+      </c>
+      <c r="F8" s="34">
+        <v>1</v>
+      </c>
+      <c r="G8" s="34">
+        <v>0</v>
+      </c>
+      <c r="H8" s="34">
+        <v>0</v>
+      </c>
+      <c r="I8" s="34">
+        <v>0</v>
+      </c>
+      <c r="J8" s="34">
+        <v>42</v>
+      </c>
+      <c r="K8" s="34">
+        <v>53</v>
+      </c>
+      <c r="L8" s="34">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A9" s="34" t="s">
+        <v>292</v>
+      </c>
+      <c r="B9" s="34">
+        <v>10</v>
+      </c>
+      <c r="C9" s="34">
+        <v>0</v>
+      </c>
+      <c r="D9" s="34">
+        <v>0</v>
+      </c>
+      <c r="E9" s="34">
+        <v>0</v>
+      </c>
+      <c r="F9" s="34">
+        <v>0</v>
+      </c>
+      <c r="G9" s="34">
+        <v>4</v>
+      </c>
+      <c r="H9" s="34">
+        <v>0</v>
+      </c>
+      <c r="I9" s="34">
+        <v>0</v>
+      </c>
+      <c r="J9" s="34">
+        <v>40</v>
+      </c>
+      <c r="K9" s="34">
+        <v>50</v>
+      </c>
+      <c r="L9" s="34">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A10" s="34" t="s">
+        <v>293</v>
+      </c>
+      <c r="B10" s="34">
+        <v>6</v>
+      </c>
+      <c r="C10" s="34">
+        <v>0</v>
+      </c>
+      <c r="D10" s="34">
+        <v>0</v>
+      </c>
+      <c r="E10" s="34">
+        <v>0</v>
+      </c>
+      <c r="F10" s="34">
+        <v>0</v>
+      </c>
+      <c r="G10" s="34">
+        <v>5</v>
+      </c>
+      <c r="H10" s="34">
+        <v>0</v>
+      </c>
+      <c r="I10" s="34">
+        <v>0</v>
+      </c>
+      <c r="J10" s="34">
+        <v>44</v>
+      </c>
+      <c r="K10" s="34">
+        <v>50</v>
+      </c>
+      <c r="L10" s="34">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A11" s="34" t="s">
+        <v>294</v>
+      </c>
+      <c r="B11" s="34">
+        <v>9</v>
+      </c>
+      <c r="C11" s="34">
+        <v>0</v>
+      </c>
+      <c r="D11" s="34">
+        <v>0</v>
+      </c>
+      <c r="E11" s="34">
+        <v>0</v>
+      </c>
+      <c r="F11" s="34">
+        <v>0</v>
+      </c>
+      <c r="G11" s="34">
+        <v>5</v>
+      </c>
+      <c r="H11" s="34">
+        <v>0</v>
+      </c>
+      <c r="I11" s="34">
+        <v>0</v>
+      </c>
+      <c r="J11" s="34">
+        <v>41</v>
+      </c>
+      <c r="K11" s="34">
+        <v>50</v>
+      </c>
+      <c r="L11" s="34">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A12" s="34" t="s">
+        <v>295</v>
+      </c>
+      <c r="B12" s="34">
+        <v>10</v>
+      </c>
+      <c r="C12" s="34">
+        <v>0</v>
+      </c>
+      <c r="D12" s="34">
+        <v>1</v>
+      </c>
+      <c r="E12" s="34">
+        <v>0</v>
+      </c>
+      <c r="F12" s="34">
+        <v>0</v>
+      </c>
+      <c r="G12" s="34">
+        <v>4</v>
+      </c>
+      <c r="H12" s="34">
+        <v>0</v>
+      </c>
+      <c r="I12" s="34">
+        <v>0</v>
+      </c>
+      <c r="J12" s="34">
+        <v>39</v>
+      </c>
+      <c r="K12" s="34">
+        <v>50</v>
+      </c>
+      <c r="L12" s="34">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A13" s="34" t="s">
+        <v>296</v>
+      </c>
+      <c r="B13" s="34">
+        <v>11</v>
+      </c>
+      <c r="C13" s="34">
+        <v>0</v>
+      </c>
+      <c r="D13" s="34">
+        <v>6</v>
+      </c>
+      <c r="E13" s="34">
+        <v>0</v>
+      </c>
+      <c r="F13" s="34">
+        <v>0</v>
+      </c>
+      <c r="G13" s="34">
+        <v>3</v>
+      </c>
+      <c r="H13" s="34">
+        <v>0</v>
+      </c>
+      <c r="I13" s="34">
+        <v>0</v>
+      </c>
+      <c r="J13" s="34">
+        <v>33</v>
+      </c>
+      <c r="K13" s="34">
+        <v>50</v>
+      </c>
+      <c r="L13" s="34">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A14" s="34" t="s">
+        <v>297</v>
+      </c>
+      <c r="B14" s="34">
+        <v>3</v>
+      </c>
+      <c r="C14" s="34">
+        <v>0</v>
+      </c>
+      <c r="D14" s="34">
+        <v>0</v>
+      </c>
+      <c r="E14" s="34">
+        <v>0</v>
+      </c>
+      <c r="F14" s="34">
+        <v>0</v>
+      </c>
+      <c r="G14" s="34">
+        <v>1</v>
+      </c>
+      <c r="H14" s="34">
+        <v>0</v>
+      </c>
+      <c r="I14" s="34">
+        <v>0</v>
+      </c>
+      <c r="J14" s="34">
+        <v>47</v>
+      </c>
+      <c r="K14" s="34">
+        <v>50</v>
+      </c>
+      <c r="L14" s="34">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A15" s="36" t="s">
+        <v>298</v>
+      </c>
+      <c r="B15" s="36">
+        <v>7</v>
+      </c>
+      <c r="C15" s="36">
+        <v>1</v>
+      </c>
+      <c r="D15" s="36">
+        <v>0</v>
+      </c>
+      <c r="E15" s="36">
+        <v>0</v>
+      </c>
+      <c r="F15" s="36">
+        <v>1</v>
+      </c>
+      <c r="G15" s="36">
+        <v>1</v>
+      </c>
+      <c r="H15" s="36">
+        <v>0</v>
+      </c>
+      <c r="I15" s="36">
+        <v>0</v>
+      </c>
+      <c r="J15" s="36">
+        <v>47</v>
+      </c>
+      <c r="K15" s="36">
+        <v>54</v>
+      </c>
+      <c r="L15" s="36">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A16" s="34" t="s">
+        <v>299</v>
+      </c>
+      <c r="B16" s="34">
+        <v>6</v>
+      </c>
+      <c r="C16" s="34">
+        <v>0</v>
+      </c>
+      <c r="D16" s="34">
+        <v>0</v>
+      </c>
+      <c r="E16" s="34">
+        <v>0</v>
+      </c>
+      <c r="F16" s="34">
+        <v>0</v>
+      </c>
+      <c r="G16" s="34">
+        <v>6</v>
+      </c>
+      <c r="H16" s="34">
+        <v>0</v>
+      </c>
+      <c r="I16" s="34">
+        <v>0</v>
+      </c>
+      <c r="J16" s="34">
+        <v>44</v>
+      </c>
+      <c r="K16" s="34">
+        <v>50</v>
+      </c>
+      <c r="L16" s="34">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A17" s="34" t="s">
+        <v>300</v>
+      </c>
+      <c r="B17" s="34">
+        <v>3</v>
+      </c>
+      <c r="C17" s="34">
+        <v>0</v>
+      </c>
+      <c r="D17" s="34">
+        <v>0</v>
+      </c>
+      <c r="E17" s="34">
+        <v>0</v>
+      </c>
+      <c r="F17" s="34">
+        <v>0</v>
+      </c>
+      <c r="G17" s="34">
+        <v>6</v>
+      </c>
+      <c r="H17" s="34">
+        <v>0</v>
+      </c>
+      <c r="I17" s="34">
+        <v>0</v>
+      </c>
+      <c r="J17" s="34">
+        <v>47</v>
+      </c>
+      <c r="K17" s="34">
+        <v>50</v>
+      </c>
+      <c r="L17" s="34">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A18" s="34" t="s">
+        <v>301</v>
+      </c>
+      <c r="B18" s="34">
+        <v>8</v>
+      </c>
+      <c r="C18" s="34">
+        <v>0</v>
+      </c>
+      <c r="D18" s="34">
+        <v>0</v>
+      </c>
+      <c r="E18" s="34">
+        <v>0</v>
+      </c>
+      <c r="F18" s="34">
+        <v>0</v>
+      </c>
+      <c r="G18" s="34">
+        <v>8</v>
+      </c>
+      <c r="H18" s="34">
+        <v>0</v>
+      </c>
+      <c r="I18" s="34">
+        <v>0</v>
+      </c>
+      <c r="J18" s="34">
+        <v>42</v>
+      </c>
+      <c r="K18" s="34">
+        <v>50</v>
+      </c>
+      <c r="L18" s="34">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A19" s="34" t="s">
+        <v>302</v>
+      </c>
+      <c r="B19" s="34">
+        <v>4</v>
+      </c>
+      <c r="C19" s="34">
+        <v>0</v>
+      </c>
+      <c r="D19" s="34">
+        <v>0</v>
+      </c>
+      <c r="E19" s="34">
+        <v>0</v>
+      </c>
+      <c r="F19" s="34">
+        <v>0</v>
+      </c>
+      <c r="G19" s="34">
+        <v>2</v>
+      </c>
+      <c r="H19" s="34">
+        <v>0</v>
+      </c>
+      <c r="I19" s="34">
+        <v>0</v>
+      </c>
+      <c r="J19" s="34">
+        <v>46</v>
+      </c>
+      <c r="K19" s="34">
+        <v>50</v>
+      </c>
+      <c r="L19" s="34">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A20" s="34" t="s">
+        <v>303</v>
+      </c>
+      <c r="B20" s="34">
+        <v>7</v>
+      </c>
+      <c r="C20" s="34">
+        <v>0</v>
+      </c>
+      <c r="D20" s="34">
+        <v>0</v>
+      </c>
+      <c r="E20" s="34">
+        <v>0</v>
+      </c>
+      <c r="F20" s="34">
+        <v>0</v>
+      </c>
+      <c r="G20" s="34">
+        <v>3</v>
+      </c>
+      <c r="H20" s="34">
+        <v>0</v>
+      </c>
+      <c r="I20" s="34">
+        <v>0</v>
+      </c>
+      <c r="J20" s="34">
+        <v>43</v>
+      </c>
+      <c r="K20" s="34">
+        <v>50</v>
+      </c>
+      <c r="L20" s="34">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A21" s="34" t="s">
+        <v>304</v>
+      </c>
+      <c r="B21" s="34">
+        <v>11</v>
+      </c>
+      <c r="C21" s="34">
+        <v>0</v>
+      </c>
+      <c r="D21" s="34">
+        <v>0</v>
+      </c>
+      <c r="E21" s="34">
+        <v>0</v>
+      </c>
+      <c r="F21" s="34">
+        <v>0</v>
+      </c>
+      <c r="G21" s="34">
+        <v>6</v>
+      </c>
+      <c r="H21" s="34">
+        <v>0</v>
+      </c>
+      <c r="I21" s="34">
+        <v>0</v>
+      </c>
+      <c r="J21" s="34">
+        <v>39</v>
+      </c>
+      <c r="K21" s="34">
+        <v>50</v>
+      </c>
+      <c r="L21" s="34">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A22" s="34" t="s">
+        <v>305</v>
+      </c>
+      <c r="B22" s="34">
+        <v>8</v>
+      </c>
+      <c r="C22" s="34">
+        <v>0</v>
+      </c>
+      <c r="D22" s="34">
+        <v>1</v>
+      </c>
+      <c r="E22" s="34">
+        <v>0</v>
+      </c>
+      <c r="F22" s="34">
+        <v>1</v>
+      </c>
+      <c r="G22" s="34">
+        <v>3</v>
+      </c>
+      <c r="H22" s="34">
+        <v>0</v>
+      </c>
+      <c r="I22" s="34">
+        <v>0</v>
+      </c>
+      <c r="J22" s="34">
+        <v>32</v>
+      </c>
+      <c r="K22" s="34">
+        <v>42</v>
+      </c>
+      <c r="L22" s="34">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A23" s="34" t="s">
+        <v>306</v>
+      </c>
+      <c r="B23" s="34">
+        <v>13</v>
+      </c>
+      <c r="C23" s="34">
+        <v>0</v>
+      </c>
+      <c r="D23" s="34">
+        <v>0</v>
+      </c>
+      <c r="E23" s="34">
+        <v>0</v>
+      </c>
+      <c r="F23" s="34">
+        <v>0</v>
+      </c>
+      <c r="G23" s="34">
+        <v>0</v>
+      </c>
+      <c r="H23" s="34">
+        <v>0</v>
+      </c>
+      <c r="I23" s="34">
+        <v>0</v>
+      </c>
+      <c r="J23" s="34">
+        <v>37</v>
+      </c>
+      <c r="K23" s="34">
+        <v>50</v>
+      </c>
+      <c r="L23" s="34">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A24" s="34" t="s">
+        <v>307</v>
+      </c>
+      <c r="B24" s="34">
+        <v>10</v>
+      </c>
+      <c r="C24" s="34">
+        <v>0</v>
+      </c>
+      <c r="D24" s="34">
+        <v>0</v>
+      </c>
+      <c r="E24" s="34">
+        <v>0</v>
+      </c>
+      <c r="F24" s="34">
+        <v>0</v>
+      </c>
+      <c r="G24" s="34">
+        <v>5</v>
+      </c>
+      <c r="H24" s="34">
+        <v>0</v>
+      </c>
+      <c r="I24" s="34">
+        <v>0</v>
+      </c>
+      <c r="J24" s="34">
+        <v>40</v>
+      </c>
+      <c r="K24" s="34">
+        <v>50</v>
+      </c>
+      <c r="L24" s="34">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A25" s="34" t="s">
+        <v>308</v>
+      </c>
+      <c r="B25" s="34">
+        <v>11</v>
+      </c>
+      <c r="C25" s="34">
+        <v>0</v>
+      </c>
+      <c r="D25" s="34">
+        <v>0</v>
+      </c>
+      <c r="E25" s="34">
+        <v>0</v>
+      </c>
+      <c r="F25" s="34">
+        <v>0</v>
+      </c>
+      <c r="G25" s="34">
+        <v>1</v>
+      </c>
+      <c r="H25" s="34">
+        <v>0</v>
+      </c>
+      <c r="I25" s="34">
+        <v>0</v>
+      </c>
+      <c r="J25" s="34">
+        <v>39</v>
+      </c>
+      <c r="K25" s="34">
+        <v>50</v>
+      </c>
+      <c r="L25" s="34">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A26" s="34" t="s">
+        <v>309</v>
+      </c>
+      <c r="B26" s="34">
+        <v>8</v>
+      </c>
+      <c r="C26" s="34">
+        <v>0</v>
+      </c>
+      <c r="D26" s="34">
+        <v>0</v>
+      </c>
+      <c r="E26" s="34">
+        <v>0</v>
+      </c>
+      <c r="F26" s="34">
+        <v>0</v>
+      </c>
+      <c r="G26" s="34">
+        <v>4</v>
+      </c>
+      <c r="H26" s="34">
+        <v>0</v>
+      </c>
+      <c r="I26" s="34">
+        <v>0</v>
+      </c>
+      <c r="J26" s="34">
+        <v>42</v>
+      </c>
+      <c r="K26" s="34">
+        <v>50</v>
+      </c>
+      <c r="L26" s="34">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A27" s="34" t="s">
+        <v>310</v>
+      </c>
+      <c r="B27" s="34">
+        <v>5</v>
+      </c>
+      <c r="C27" s="34">
+        <v>0</v>
+      </c>
+      <c r="D27" s="34">
+        <v>0</v>
+      </c>
+      <c r="E27" s="34">
+        <v>0</v>
+      </c>
+      <c r="F27" s="34">
+        <v>1</v>
+      </c>
+      <c r="G27" s="34">
+        <v>3</v>
+      </c>
+      <c r="H27" s="34">
+        <v>0</v>
+      </c>
+      <c r="I27" s="34">
+        <v>0</v>
+      </c>
+      <c r="J27" s="34">
+        <v>24</v>
+      </c>
+      <c r="K27" s="34">
+        <v>30</v>
+      </c>
+      <c r="L27" s="34">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A28" s="34" t="s">
+        <v>311</v>
+      </c>
+      <c r="B28" s="34">
+        <v>11</v>
+      </c>
+      <c r="C28" s="34">
+        <v>0</v>
+      </c>
+      <c r="D28" s="34">
+        <v>1</v>
+      </c>
+      <c r="E28" s="34">
+        <v>0</v>
+      </c>
+      <c r="F28" s="34">
+        <v>0</v>
+      </c>
+      <c r="G28" s="34">
+        <v>4</v>
+      </c>
+      <c r="H28" s="34">
+        <v>0</v>
+      </c>
+      <c r="I28" s="34">
+        <v>0</v>
+      </c>
+      <c r="J28" s="34">
+        <v>38</v>
+      </c>
+      <c r="K28" s="34">
+        <v>50</v>
+      </c>
+      <c r="L28" s="34">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A29" s="34" t="s">
+        <v>312</v>
+      </c>
+      <c r="B29" s="34">
+        <v>6</v>
+      </c>
+      <c r="C29" s="34">
+        <v>0</v>
+      </c>
+      <c r="D29" s="34">
+        <v>1</v>
+      </c>
+      <c r="E29" s="34">
+        <v>0</v>
+      </c>
+      <c r="F29" s="34">
+        <v>0</v>
+      </c>
+      <c r="G29" s="34">
+        <v>4</v>
+      </c>
+      <c r="H29" s="34">
+        <v>0</v>
+      </c>
+      <c r="I29" s="34">
+        <v>0</v>
+      </c>
+      <c r="J29" s="34">
+        <v>43</v>
+      </c>
+      <c r="K29" s="34">
+        <v>50</v>
+      </c>
+      <c r="L29" s="34">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A30" s="34" t="s">
+        <v>313</v>
+      </c>
+      <c r="B30" s="34">
+        <v>14</v>
+      </c>
+      <c r="C30" s="34">
+        <v>0</v>
+      </c>
+      <c r="D30" s="34">
+        <v>1</v>
+      </c>
+      <c r="E30" s="34">
+        <v>0</v>
+      </c>
+      <c r="F30" s="34">
+        <v>0</v>
+      </c>
+      <c r="G30" s="34">
+        <v>1</v>
+      </c>
+      <c r="H30" s="34">
+        <v>0</v>
+      </c>
+      <c r="I30" s="34">
+        <v>0</v>
+      </c>
+      <c r="J30" s="34">
+        <v>35</v>
+      </c>
+      <c r="K30" s="34">
+        <v>50</v>
+      </c>
+      <c r="L30" s="34">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A31" s="34" t="s">
+        <v>314</v>
+      </c>
+      <c r="B31" s="34">
+        <v>17</v>
+      </c>
+      <c r="C31" s="34">
+        <v>0</v>
+      </c>
+      <c r="D31" s="34">
+        <v>0</v>
+      </c>
+      <c r="E31" s="34">
+        <v>0</v>
+      </c>
+      <c r="F31" s="34">
+        <v>0</v>
+      </c>
+      <c r="G31" s="34">
+        <v>3</v>
+      </c>
+      <c r="H31" s="34">
+        <v>0</v>
+      </c>
+      <c r="I31" s="34">
+        <v>0</v>
+      </c>
+      <c r="J31" s="34">
+        <v>33</v>
+      </c>
+      <c r="K31" s="34">
+        <v>50</v>
+      </c>
+      <c r="L31" s="34">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A32" s="34" t="s">
+        <v>315</v>
+      </c>
+      <c r="B32" s="34">
+        <v>8</v>
+      </c>
+      <c r="C32" s="34">
+        <v>0</v>
+      </c>
+      <c r="D32" s="34">
+        <v>2</v>
+      </c>
+      <c r="E32" s="34">
+        <v>0</v>
+      </c>
+      <c r="F32" s="34">
+        <v>0</v>
+      </c>
+      <c r="G32" s="34">
+        <v>2</v>
+      </c>
+      <c r="H32" s="34">
+        <v>0</v>
+      </c>
+      <c r="I32" s="34">
+        <v>0</v>
+      </c>
+      <c r="J32" s="34">
+        <v>40</v>
+      </c>
+      <c r="K32" s="34">
+        <v>50</v>
+      </c>
+      <c r="L32" s="34">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A33" s="34" t="s">
+        <v>316</v>
+      </c>
+      <c r="B33" s="34">
+        <v>7</v>
+      </c>
+      <c r="C33" s="34">
+        <v>0</v>
+      </c>
+      <c r="D33" s="34">
+        <v>0</v>
+      </c>
+      <c r="E33" s="34">
+        <v>0</v>
+      </c>
+      <c r="F33" s="34">
+        <v>1</v>
+      </c>
+      <c r="G33" s="34">
+        <v>2</v>
+      </c>
+      <c r="H33" s="34">
+        <v>0</v>
+      </c>
+      <c r="I33" s="34">
+        <v>0</v>
+      </c>
+      <c r="J33" s="34">
+        <v>48</v>
+      </c>
+      <c r="K33" s="34">
+        <v>56</v>
+      </c>
+      <c r="L33" s="34">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A34" s="34" t="s">
+        <v>317</v>
+      </c>
+      <c r="B34" s="34">
+        <v>15</v>
+      </c>
+      <c r="C34" s="34">
+        <v>0</v>
+      </c>
+      <c r="D34" s="34">
+        <v>2</v>
+      </c>
+      <c r="E34" s="34">
+        <v>0</v>
+      </c>
+      <c r="F34" s="34">
+        <v>0</v>
+      </c>
+      <c r="G34" s="34">
+        <v>3</v>
+      </c>
+      <c r="H34" s="34">
+        <v>0</v>
+      </c>
+      <c r="I34" s="34">
+        <v>0</v>
+      </c>
+      <c r="J34" s="34">
+        <v>33</v>
+      </c>
+      <c r="K34" s="34">
+        <v>50</v>
+      </c>
+      <c r="L34" s="34">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A35" s="34" t="s">
+        <v>318</v>
+      </c>
+      <c r="B35" s="34">
+        <v>11</v>
+      </c>
+      <c r="C35" s="34">
+        <v>0</v>
+      </c>
+      <c r="D35" s="34">
+        <v>2</v>
+      </c>
+      <c r="E35" s="34">
+        <v>0</v>
+      </c>
+      <c r="F35" s="34">
+        <v>0</v>
+      </c>
+      <c r="G35" s="34">
+        <v>2</v>
+      </c>
+      <c r="H35" s="34">
+        <v>0</v>
+      </c>
+      <c r="I35" s="34">
+        <v>0</v>
+      </c>
+      <c r="J35" s="34">
+        <v>37</v>
+      </c>
+      <c r="K35" s="34">
+        <v>50</v>
+      </c>
+      <c r="L35" s="34">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A36" s="34" t="s">
+        <v>319</v>
+      </c>
+      <c r="B36" s="34">
+        <v>12</v>
+      </c>
+      <c r="C36" s="34">
+        <v>0</v>
+      </c>
+      <c r="D36" s="34">
+        <v>0</v>
+      </c>
+      <c r="E36" s="34">
+        <v>0</v>
+      </c>
+      <c r="F36" s="34">
+        <v>0</v>
+      </c>
+      <c r="G36" s="34">
+        <v>0</v>
+      </c>
+      <c r="H36" s="34">
+        <v>0</v>
+      </c>
+      <c r="I36" s="34">
+        <v>0</v>
+      </c>
+      <c r="J36" s="34">
+        <v>38</v>
+      </c>
+      <c r="K36" s="34">
+        <v>50</v>
+      </c>
+      <c r="L36" s="34">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A37" s="34" t="s">
+        <v>320</v>
+      </c>
+      <c r="B37" s="34">
+        <v>10</v>
+      </c>
+      <c r="C37" s="34">
+        <v>0</v>
+      </c>
+      <c r="D37" s="34">
+        <v>0</v>
+      </c>
+      <c r="E37" s="34">
+        <v>0</v>
+      </c>
+      <c r="F37" s="34">
+        <v>0</v>
+      </c>
+      <c r="G37" s="34">
+        <v>2</v>
+      </c>
+      <c r="H37" s="34">
+        <v>0</v>
+      </c>
+      <c r="I37" s="34">
+        <v>0</v>
+      </c>
+      <c r="J37" s="34">
+        <v>40</v>
+      </c>
+      <c r="K37" s="34">
+        <v>50</v>
+      </c>
+      <c r="L37" s="34">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A38" s="34" t="s">
+        <v>321</v>
+      </c>
+      <c r="B38" s="34">
+        <v>2</v>
+      </c>
+      <c r="C38" s="34">
+        <v>0</v>
+      </c>
+      <c r="D38" s="34">
+        <v>4</v>
+      </c>
+      <c r="E38" s="34">
+        <v>0</v>
+      </c>
+      <c r="F38" s="34">
+        <v>0</v>
+      </c>
+      <c r="G38" s="34">
+        <v>3</v>
+      </c>
+      <c r="H38" s="34">
+        <v>0</v>
+      </c>
+      <c r="I38" s="34">
+        <v>0</v>
+      </c>
+      <c r="J38" s="34">
+        <v>44</v>
+      </c>
+      <c r="K38" s="34">
+        <v>50</v>
+      </c>
+      <c r="L38" s="34">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A39" s="34" t="s">
+        <v>322</v>
+      </c>
+      <c r="B39" s="34">
+        <v>9</v>
+      </c>
+      <c r="C39" s="34">
+        <v>0</v>
+      </c>
+      <c r="D39" s="34">
+        <v>2</v>
+      </c>
+      <c r="E39" s="34">
+        <v>0</v>
+      </c>
+      <c r="F39" s="34">
+        <v>1</v>
+      </c>
+      <c r="G39" s="34">
+        <v>1</v>
+      </c>
+      <c r="H39" s="34">
+        <v>0</v>
+      </c>
+      <c r="I39" s="34">
+        <v>0</v>
+      </c>
+      <c r="J39" s="34">
+        <v>45</v>
+      </c>
+      <c r="K39" s="34">
+        <v>57</v>
+      </c>
+      <c r="L39" s="34">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A40" s="34" t="s">
+        <v>323</v>
+      </c>
+      <c r="B40" s="34">
+        <v>2</v>
+      </c>
+      <c r="C40" s="34">
+        <v>0</v>
+      </c>
+      <c r="D40" s="34">
+        <v>0</v>
+      </c>
+      <c r="E40" s="34">
+        <v>0</v>
+      </c>
+      <c r="F40" s="34">
+        <v>0</v>
+      </c>
+      <c r="G40" s="34">
+        <v>2</v>
+      </c>
+      <c r="H40" s="34">
+        <v>0</v>
+      </c>
+      <c r="I40" s="34">
+        <v>0</v>
+      </c>
+      <c r="J40" s="34">
+        <v>48</v>
+      </c>
+      <c r="K40" s="34">
+        <v>50</v>
+      </c>
+      <c r="L40" s="34">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A41" s="34" t="s">
+        <v>324</v>
+      </c>
+      <c r="B41" s="34">
+        <v>9</v>
+      </c>
+      <c r="C41" s="34">
+        <v>0</v>
+      </c>
+      <c r="D41" s="34">
+        <v>1</v>
+      </c>
+      <c r="E41" s="34">
+        <v>0</v>
+      </c>
+      <c r="F41" s="34">
+        <v>0</v>
+      </c>
+      <c r="G41" s="34">
+        <v>8</v>
+      </c>
+      <c r="H41" s="34">
+        <v>0</v>
+      </c>
+      <c r="I41" s="34">
+        <v>0</v>
+      </c>
+      <c r="J41" s="34">
+        <v>40</v>
+      </c>
+      <c r="K41" s="34">
+        <v>50</v>
+      </c>
+      <c r="L41" s="34">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A42" s="34" t="s">
+        <v>325</v>
+      </c>
+      <c r="B42" s="34">
+        <v>5</v>
+      </c>
+      <c r="C42" s="34">
+        <v>0</v>
+      </c>
+      <c r="D42" s="34">
+        <v>0</v>
+      </c>
+      <c r="E42" s="34">
+        <v>0</v>
+      </c>
+      <c r="F42" s="34">
+        <v>0</v>
+      </c>
+      <c r="G42" s="34">
+        <v>9</v>
+      </c>
+      <c r="H42" s="34">
+        <v>0</v>
+      </c>
+      <c r="I42" s="34">
+        <v>0</v>
+      </c>
+      <c r="J42" s="34">
+        <v>45</v>
+      </c>
+      <c r="K42" s="34">
+        <v>50</v>
+      </c>
+      <c r="L42" s="34">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A43" s="34" t="s">
+        <v>326</v>
+      </c>
+      <c r="B43" s="34">
+        <v>7</v>
+      </c>
+      <c r="C43" s="34">
+        <v>0</v>
+      </c>
+      <c r="D43" s="34">
+        <v>0</v>
+      </c>
+      <c r="E43" s="34">
+        <v>0</v>
+      </c>
+      <c r="F43" s="34">
+        <v>0</v>
+      </c>
+      <c r="G43" s="34">
+        <v>5</v>
+      </c>
+      <c r="H43" s="34">
+        <v>0</v>
+      </c>
+      <c r="I43" s="34">
+        <v>0</v>
+      </c>
+      <c r="J43" s="34">
+        <v>43</v>
+      </c>
+      <c r="K43" s="34">
+        <v>50</v>
+      </c>
+      <c r="L43" s="34">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A44" s="34" t="s">
+        <v>327</v>
+      </c>
+      <c r="B44" s="34">
+        <v>15</v>
+      </c>
+      <c r="C44" s="34">
+        <v>0</v>
+      </c>
+      <c r="D44" s="34">
+        <v>0</v>
+      </c>
+      <c r="E44" s="34">
+        <v>0</v>
+      </c>
+      <c r="F44" s="34">
+        <v>1</v>
+      </c>
+      <c r="G44" s="34">
+        <v>4</v>
+      </c>
+      <c r="H44" s="34">
+        <v>0</v>
+      </c>
+      <c r="I44" s="34">
+        <v>0</v>
+      </c>
+      <c r="J44" s="34">
+        <v>44</v>
+      </c>
+      <c r="K44" s="34">
+        <v>60</v>
+      </c>
+      <c r="L44" s="34">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A45" s="34" t="s">
+        <v>328</v>
+      </c>
+      <c r="B45" s="34">
+        <v>6</v>
+      </c>
+      <c r="C45" s="34">
+        <v>0</v>
+      </c>
+      <c r="D45" s="34">
+        <v>0</v>
+      </c>
+      <c r="E45" s="34">
+        <v>0</v>
+      </c>
+      <c r="F45" s="34">
+        <v>0</v>
+      </c>
+      <c r="G45" s="34">
+        <v>1</v>
+      </c>
+      <c r="H45" s="34">
+        <v>0</v>
+      </c>
+      <c r="I45" s="34">
+        <v>0</v>
+      </c>
+      <c r="J45" s="34">
+        <v>44</v>
+      </c>
+      <c r="K45" s="34">
+        <v>50</v>
+      </c>
+      <c r="L45" s="34">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A46" s="34" t="s">
+        <v>329</v>
+      </c>
+      <c r="B46" s="34">
+        <v>5</v>
+      </c>
+      <c r="C46" s="34">
+        <v>0</v>
+      </c>
+      <c r="D46" s="34">
+        <v>0</v>
+      </c>
+      <c r="E46" s="34">
+        <v>0</v>
+      </c>
+      <c r="F46" s="34">
+        <v>0</v>
+      </c>
+      <c r="G46" s="34">
+        <v>5</v>
+      </c>
+      <c r="H46" s="34">
+        <v>0</v>
+      </c>
+      <c r="I46" s="34">
+        <v>0</v>
+      </c>
+      <c r="J46" s="34">
+        <v>45</v>
+      </c>
+      <c r="K46" s="34">
+        <v>50</v>
+      </c>
+      <c r="L46" s="34">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="47" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A47" s="34" t="s">
+        <v>330</v>
+      </c>
+      <c r="B47" s="34">
+        <v>9</v>
+      </c>
+      <c r="C47" s="34">
+        <v>0</v>
+      </c>
+      <c r="D47" s="34">
+        <v>0</v>
+      </c>
+      <c r="E47" s="34">
+        <v>0</v>
+      </c>
+      <c r="F47" s="34">
+        <v>0</v>
+      </c>
+      <c r="G47" s="34">
+        <v>2</v>
+      </c>
+      <c r="H47" s="34">
+        <v>0</v>
+      </c>
+      <c r="I47" s="34">
+        <v>0</v>
+      </c>
+      <c r="J47" s="34">
+        <v>41</v>
+      </c>
+      <c r="K47" s="34">
+        <v>50</v>
+      </c>
+      <c r="L47" s="34">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A48" s="34" t="s">
+        <v>331</v>
+      </c>
+      <c r="B48" s="34">
+        <v>7</v>
+      </c>
+      <c r="C48" s="34">
+        <v>0</v>
+      </c>
+      <c r="D48" s="34">
+        <v>0</v>
+      </c>
+      <c r="E48" s="34">
+        <v>0</v>
+      </c>
+      <c r="F48" s="34">
+        <v>0</v>
+      </c>
+      <c r="G48" s="34">
+        <v>1</v>
+      </c>
+      <c r="H48" s="34">
+        <v>0</v>
+      </c>
+      <c r="I48" s="34">
+        <v>0</v>
+      </c>
+      <c r="J48" s="34">
+        <v>43</v>
+      </c>
+      <c r="K48" s="34">
+        <v>50</v>
+      </c>
+      <c r="L48" s="34">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="49" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A49" s="34" t="s">
+        <v>332</v>
+      </c>
+      <c r="B49" s="34">
+        <v>6</v>
+      </c>
+      <c r="C49" s="34">
+        <v>0</v>
+      </c>
+      <c r="D49" s="34">
+        <v>0</v>
+      </c>
+      <c r="E49" s="34">
+        <v>0</v>
+      </c>
+      <c r="F49" s="34">
+        <v>0</v>
+      </c>
+      <c r="G49" s="34">
+        <v>4</v>
+      </c>
+      <c r="H49" s="34">
+        <v>0</v>
+      </c>
+      <c r="I49" s="34">
+        <v>0</v>
+      </c>
+      <c r="J49" s="34">
+        <v>44</v>
+      </c>
+      <c r="K49" s="34">
+        <v>50</v>
+      </c>
+      <c r="L49" s="34">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="50" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A50" s="34" t="s">
+        <v>333</v>
+      </c>
+      <c r="B50" s="34">
+        <v>9</v>
+      </c>
+      <c r="C50" s="34">
+        <v>0</v>
+      </c>
+      <c r="D50" s="34">
+        <v>0</v>
+      </c>
+      <c r="E50" s="34">
+        <v>0</v>
+      </c>
+      <c r="F50" s="34">
+        <v>0</v>
+      </c>
+      <c r="G50" s="34">
+        <v>2</v>
+      </c>
+      <c r="H50" s="34">
+        <v>0</v>
+      </c>
+      <c r="I50" s="34">
+        <v>0</v>
+      </c>
+      <c r="J50" s="34">
+        <v>41</v>
+      </c>
+      <c r="K50" s="34">
+        <v>50</v>
+      </c>
+      <c r="L50" s="34">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="51" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A51" s="34" t="s">
+        <v>334</v>
+      </c>
+      <c r="B51" s="34">
+        <v>2</v>
+      </c>
+      <c r="C51" s="34">
+        <v>0</v>
+      </c>
+      <c r="D51" s="34">
+        <v>1</v>
+      </c>
+      <c r="E51" s="34">
+        <v>0</v>
+      </c>
+      <c r="F51" s="34">
+        <v>1</v>
+      </c>
+      <c r="G51" s="34">
+        <v>2</v>
+      </c>
+      <c r="H51" s="34">
+        <v>0</v>
+      </c>
+      <c r="I51" s="34">
+        <v>0</v>
+      </c>
+      <c r="J51" s="34">
+        <v>25</v>
+      </c>
+      <c r="K51" s="34">
+        <v>29</v>
+      </c>
+      <c r="L51" s="34">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="52" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A52" s="34" t="s">
+        <v>335</v>
+      </c>
+      <c r="B52" s="34">
+        <v>5</v>
+      </c>
+      <c r="C52" s="34">
+        <v>0</v>
+      </c>
+      <c r="D52" s="34">
+        <v>0</v>
+      </c>
+      <c r="E52" s="34">
+        <v>0</v>
+      </c>
+      <c r="F52" s="34">
+        <v>0</v>
+      </c>
+      <c r="G52" s="34">
+        <v>0</v>
+      </c>
+      <c r="H52" s="34">
+        <v>0</v>
+      </c>
+      <c r="I52" s="34">
+        <v>0</v>
+      </c>
+      <c r="J52" s="34">
+        <v>45</v>
+      </c>
+      <c r="K52" s="34">
+        <v>50</v>
+      </c>
+      <c r="L52" s="34">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="53" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A53" s="34" t="s">
+        <v>336</v>
+      </c>
+      <c r="B53" s="34">
+        <v>9</v>
+      </c>
+      <c r="C53" s="34">
+        <v>0</v>
+      </c>
+      <c r="D53" s="34">
+        <v>0</v>
+      </c>
+      <c r="E53" s="34">
+        <v>0</v>
+      </c>
+      <c r="F53" s="34">
+        <v>0</v>
+      </c>
+      <c r="G53" s="34">
+        <v>0</v>
+      </c>
+      <c r="H53" s="34">
+        <v>0</v>
+      </c>
+      <c r="I53" s="34">
+        <v>0</v>
+      </c>
+      <c r="J53" s="34">
+        <v>41</v>
+      </c>
+      <c r="K53" s="34">
+        <v>50</v>
+      </c>
+      <c r="L53" s="34">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="54" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A54" s="34" t="s">
+        <v>337</v>
+      </c>
+      <c r="B54" s="34">
+        <v>6</v>
+      </c>
+      <c r="C54" s="34">
+        <v>0</v>
+      </c>
+      <c r="D54" s="34">
+        <v>0</v>
+      </c>
+      <c r="E54" s="34">
+        <v>0</v>
+      </c>
+      <c r="F54" s="34">
+        <v>0</v>
+      </c>
+      <c r="G54" s="34">
+        <v>1</v>
+      </c>
+      <c r="H54" s="34">
+        <v>0</v>
+      </c>
+      <c r="I54" s="34">
+        <v>0</v>
+      </c>
+      <c r="J54" s="34">
+        <v>44</v>
+      </c>
+      <c r="K54" s="34">
+        <v>50</v>
+      </c>
+      <c r="L54" s="34">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="55" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A55" s="34" t="s">
+        <v>338</v>
+      </c>
+      <c r="B55" s="34">
+        <v>4</v>
+      </c>
+      <c r="C55" s="34">
+        <v>0</v>
+      </c>
+      <c r="D55" s="34">
+        <v>0</v>
+      </c>
+      <c r="E55" s="34">
+        <v>0</v>
+      </c>
+      <c r="F55" s="34">
+        <v>0</v>
+      </c>
+      <c r="G55" s="34">
+        <v>6</v>
+      </c>
+      <c r="H55" s="34">
+        <v>0</v>
+      </c>
+      <c r="I55" s="34">
+        <v>0</v>
+      </c>
+      <c r="J55" s="34">
+        <v>46</v>
+      </c>
+      <c r="K55" s="34">
+        <v>50</v>
+      </c>
+      <c r="L55" s="34">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="56" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A56" s="34" t="s">
+        <v>339</v>
+      </c>
+      <c r="B56" s="34">
+        <v>6</v>
+      </c>
+      <c r="C56" s="34">
+        <v>0</v>
+      </c>
+      <c r="D56" s="34">
+        <v>0</v>
+      </c>
+      <c r="E56" s="34">
+        <v>0</v>
+      </c>
+      <c r="F56" s="34">
+        <v>0</v>
+      </c>
+      <c r="G56" s="34">
+        <v>2</v>
+      </c>
+      <c r="H56" s="34">
+        <v>0</v>
+      </c>
+      <c r="I56" s="34">
+        <v>0</v>
+      </c>
+      <c r="J56" s="34">
+        <v>44</v>
+      </c>
+      <c r="K56" s="34">
+        <v>50</v>
+      </c>
+      <c r="L56" s="34">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="57" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A57" s="34" t="s">
+        <v>340</v>
+      </c>
+      <c r="B57" s="34">
+        <v>4</v>
+      </c>
+      <c r="C57" s="34">
+        <v>0</v>
+      </c>
+      <c r="D57" s="34">
+        <v>2</v>
+      </c>
+      <c r="E57" s="34">
+        <v>0</v>
+      </c>
+      <c r="F57" s="34">
+        <v>1</v>
+      </c>
+      <c r="G57" s="34">
+        <v>1</v>
+      </c>
+      <c r="H57" s="34">
+        <v>0</v>
+      </c>
+      <c r="I57" s="34">
+        <v>0</v>
+      </c>
+      <c r="J57" s="34">
+        <v>46</v>
+      </c>
+      <c r="K57" s="34">
+        <v>53</v>
+      </c>
+      <c r="L57" s="34">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="58" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A58" s="34" t="s">
+        <v>341</v>
+      </c>
+      <c r="B58" s="34">
+        <v>4</v>
+      </c>
+      <c r="C58" s="34">
+        <v>0</v>
+      </c>
+      <c r="D58" s="34">
+        <v>0</v>
+      </c>
+      <c r="E58" s="34">
+        <v>0</v>
+      </c>
+      <c r="F58" s="34">
+        <v>0</v>
+      </c>
+      <c r="G58" s="34">
+        <v>5</v>
+      </c>
+      <c r="H58" s="34">
+        <v>0</v>
+      </c>
+      <c r="I58" s="34">
+        <v>0</v>
+      </c>
+      <c r="J58" s="34">
+        <v>46</v>
+      </c>
+      <c r="K58" s="34">
+        <v>50</v>
+      </c>
+      <c r="L58" s="34">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="59" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A59" s="34" t="s">
+        <v>342</v>
+      </c>
+      <c r="B59" s="34">
+        <v>11</v>
+      </c>
+      <c r="C59" s="34">
+        <v>0</v>
+      </c>
+      <c r="D59" s="34">
+        <v>0</v>
+      </c>
+      <c r="E59" s="34">
+        <v>0</v>
+      </c>
+      <c r="F59" s="34">
+        <v>0</v>
+      </c>
+      <c r="G59" s="34">
+        <v>6</v>
+      </c>
+      <c r="H59" s="34">
+        <v>0</v>
+      </c>
+      <c r="I59" s="34">
+        <v>0</v>
+      </c>
+      <c r="J59" s="34">
+        <v>39</v>
+      </c>
+      <c r="K59" s="34">
+        <v>50</v>
+      </c>
+      <c r="L59" s="34">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="60" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A60" s="34" t="s">
+        <v>343</v>
+      </c>
+      <c r="B60" s="34">
+        <v>20</v>
+      </c>
+      <c r="C60" s="34">
+        <v>0</v>
+      </c>
+      <c r="D60" s="34">
+        <v>0</v>
+      </c>
+      <c r="E60" s="34">
+        <v>0</v>
+      </c>
+      <c r="F60" s="34">
+        <v>0</v>
+      </c>
+      <c r="G60" s="34">
+        <v>6</v>
+      </c>
+      <c r="H60" s="34">
+        <v>0</v>
+      </c>
+      <c r="I60" s="34">
+        <v>0</v>
+      </c>
+      <c r="J60" s="34">
+        <v>30</v>
+      </c>
+      <c r="K60" s="34">
+        <v>50</v>
+      </c>
+      <c r="L60" s="34">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="61" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A61" s="34" t="s">
+        <v>344</v>
+      </c>
+      <c r="B61" s="34">
+        <v>12</v>
+      </c>
+      <c r="C61" s="34">
+        <v>1</v>
+      </c>
+      <c r="D61" s="34">
+        <v>0</v>
+      </c>
+      <c r="E61" s="34">
+        <v>0</v>
+      </c>
+      <c r="F61" s="34">
+        <v>1</v>
+      </c>
+      <c r="G61" s="34">
+        <v>7</v>
+      </c>
+      <c r="H61" s="34">
+        <v>0</v>
+      </c>
+      <c r="I61" s="34">
+        <v>0</v>
+      </c>
+      <c r="J61" s="34">
+        <v>35</v>
+      </c>
+      <c r="K61" s="34">
+        <v>47</v>
+      </c>
+      <c r="L61" s="34">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="62" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A62" s="34" t="s">
+        <v>345</v>
+      </c>
+      <c r="B62" s="34">
+        <v>11</v>
+      </c>
+      <c r="C62" s="34">
+        <v>0</v>
+      </c>
+      <c r="D62" s="34">
+        <v>0</v>
+      </c>
+      <c r="E62" s="34">
+        <v>0</v>
+      </c>
+      <c r="F62" s="34">
+        <v>0</v>
+      </c>
+      <c r="G62" s="34">
+        <v>4</v>
+      </c>
+      <c r="H62" s="34">
+        <v>0</v>
+      </c>
+      <c r="I62" s="34">
+        <v>0</v>
+      </c>
+      <c r="J62" s="34">
+        <v>39</v>
+      </c>
+      <c r="K62" s="34">
+        <v>50</v>
+      </c>
+      <c r="L62" s="34">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="63" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A63" s="34" t="s">
+        <v>346</v>
+      </c>
+      <c r="B63" s="34">
+        <v>7</v>
+      </c>
+      <c r="C63" s="34">
+        <v>0</v>
+      </c>
+      <c r="D63" s="34">
+        <v>4</v>
+      </c>
+      <c r="E63" s="34">
+        <v>0</v>
+      </c>
+      <c r="F63" s="34">
+        <v>0</v>
+      </c>
+      <c r="G63" s="34">
+        <v>5</v>
+      </c>
+      <c r="H63" s="34">
+        <v>0</v>
+      </c>
+      <c r="I63" s="34">
+        <v>0</v>
+      </c>
+      <c r="J63" s="34">
+        <v>39</v>
+      </c>
+      <c r="K63" s="34">
+        <v>50</v>
+      </c>
+      <c r="L63" s="34">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="64" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A64" s="34" t="s">
+        <v>347</v>
+      </c>
+      <c r="B64" s="34">
+        <v>12</v>
+      </c>
+      <c r="C64" s="34">
+        <v>0</v>
+      </c>
+      <c r="D64" s="34">
+        <v>2</v>
+      </c>
+      <c r="E64" s="34">
+        <v>0</v>
+      </c>
+      <c r="F64" s="34">
+        <v>0</v>
+      </c>
+      <c r="G64" s="34">
+        <v>5</v>
+      </c>
+      <c r="H64" s="34">
+        <v>0</v>
+      </c>
+      <c r="I64" s="34">
+        <v>0</v>
+      </c>
+      <c r="J64" s="34">
+        <v>36</v>
+      </c>
+      <c r="K64" s="34">
+        <v>50</v>
+      </c>
+      <c r="L64" s="34">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="65" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A65" s="34" t="s">
+        <v>348</v>
+      </c>
+      <c r="B65" s="34">
+        <v>4</v>
+      </c>
+      <c r="C65" s="34">
+        <v>0</v>
+      </c>
+      <c r="D65" s="34">
+        <v>1</v>
+      </c>
+      <c r="E65" s="34">
+        <v>0</v>
+      </c>
+      <c r="F65" s="34">
+        <v>0</v>
+      </c>
+      <c r="G65" s="34">
+        <v>3</v>
+      </c>
+      <c r="H65" s="34">
+        <v>0</v>
+      </c>
+      <c r="I65" s="34">
+        <v>0</v>
+      </c>
+      <c r="J65" s="34">
+        <v>45</v>
+      </c>
+      <c r="K65" s="34">
+        <v>50</v>
+      </c>
+      <c r="L65" s="34">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="66" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A66" s="34" t="s">
+        <v>349</v>
+      </c>
+      <c r="B66" s="34">
+        <v>8</v>
+      </c>
+      <c r="C66" s="34">
+        <v>0</v>
+      </c>
+      <c r="D66" s="34">
+        <v>0</v>
+      </c>
+      <c r="E66" s="34">
+        <v>0</v>
+      </c>
+      <c r="F66" s="34">
+        <v>0</v>
+      </c>
+      <c r="G66" s="34">
+        <v>2</v>
+      </c>
+      <c r="H66" s="34">
+        <v>0</v>
+      </c>
+      <c r="I66" s="34">
+        <v>0</v>
+      </c>
+      <c r="J66" s="34">
+        <v>42</v>
+      </c>
+      <c r="K66" s="34">
+        <v>50</v>
+      </c>
+      <c r="L66" s="34">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="67" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A67" s="34" t="s">
+        <v>350</v>
+      </c>
+      <c r="B67" s="34">
+        <v>10</v>
+      </c>
+      <c r="C67" s="34">
+        <v>0</v>
+      </c>
+      <c r="D67" s="34">
+        <v>1</v>
+      </c>
+      <c r="E67" s="34">
+        <v>0</v>
+      </c>
+      <c r="F67" s="34">
+        <v>0</v>
+      </c>
+      <c r="G67" s="34">
+        <v>7</v>
+      </c>
+      <c r="H67" s="34">
+        <v>0</v>
+      </c>
+      <c r="I67" s="34">
+        <v>0</v>
+      </c>
+      <c r="J67" s="34">
+        <v>39</v>
+      </c>
+      <c r="K67" s="34">
+        <v>50</v>
+      </c>
+      <c r="L67" s="34">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="68" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A68" s="34" t="s">
+        <v>351</v>
+      </c>
+      <c r="B68" s="34">
+        <v>11</v>
+      </c>
+      <c r="C68" s="34">
+        <v>0</v>
+      </c>
+      <c r="D68" s="34">
+        <v>1</v>
+      </c>
+      <c r="E68" s="34">
+        <v>0</v>
+      </c>
+      <c r="F68" s="34">
+        <v>0</v>
+      </c>
+      <c r="G68" s="34">
+        <v>5</v>
+      </c>
+      <c r="H68" s="34">
+        <v>0</v>
+      </c>
+      <c r="I68" s="34">
+        <v>0</v>
+      </c>
+      <c r="J68" s="34">
+        <v>38</v>
+      </c>
+      <c r="K68" s="34">
+        <v>50</v>
+      </c>
+      <c r="L68" s="34">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="69" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A69" s="34" t="s">
+        <v>352</v>
+      </c>
+      <c r="B69" s="34">
+        <v>4</v>
+      </c>
+      <c r="C69" s="34">
+        <v>0</v>
+      </c>
+      <c r="D69" s="34">
+        <v>0</v>
+      </c>
+      <c r="E69" s="34">
+        <v>0</v>
+      </c>
+      <c r="F69" s="34">
+        <v>0</v>
+      </c>
+      <c r="G69" s="34">
+        <v>4</v>
+      </c>
+      <c r="H69" s="34">
+        <v>0</v>
+      </c>
+      <c r="I69" s="34">
+        <v>0</v>
+      </c>
+      <c r="J69" s="34">
+        <v>46</v>
+      </c>
+      <c r="K69" s="34">
+        <v>50</v>
+      </c>
+      <c r="L69" s="34">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="70" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A70" s="34" t="s">
+        <v>353</v>
+      </c>
+      <c r="B70" s="34">
+        <v>6</v>
+      </c>
+      <c r="C70" s="34">
+        <v>1</v>
+      </c>
+      <c r="D70" s="34">
+        <v>0</v>
+      </c>
+      <c r="E70" s="34">
+        <v>0</v>
+      </c>
+      <c r="F70" s="34">
+        <v>1</v>
+      </c>
+      <c r="G70" s="34">
+        <v>5</v>
+      </c>
+      <c r="H70" s="34">
+        <v>0</v>
+      </c>
+      <c r="I70" s="34">
+        <v>0</v>
+      </c>
+      <c r="J70" s="34">
+        <v>34</v>
+      </c>
+      <c r="K70" s="34">
+        <v>40</v>
+      </c>
+      <c r="L70" s="34">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="71" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A71" s="34" t="s">
+        <v>354</v>
+      </c>
+      <c r="B71" s="34">
+        <v>5</v>
+      </c>
+      <c r="C71" s="34">
+        <v>0</v>
+      </c>
+      <c r="D71" s="34">
+        <v>2</v>
+      </c>
+      <c r="E71" s="34">
+        <v>0</v>
+      </c>
+      <c r="F71" s="34">
+        <v>3</v>
+      </c>
+      <c r="G71" s="34">
+        <v>10</v>
+      </c>
+      <c r="H71" s="34">
+        <v>0</v>
+      </c>
+      <c r="I71" s="34">
+        <v>0</v>
+      </c>
+      <c r="J71" s="34">
+        <v>40</v>
+      </c>
+      <c r="K71" s="34">
+        <v>50</v>
+      </c>
+      <c r="L71" s="34">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="72" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A72" s="34" t="s">
+        <v>355</v>
+      </c>
+      <c r="B72" s="34">
+        <v>5</v>
+      </c>
+      <c r="C72" s="34">
+        <v>1</v>
+      </c>
+      <c r="D72" s="34">
+        <v>0</v>
+      </c>
+      <c r="E72" s="34">
+        <v>0</v>
+      </c>
+      <c r="F72" s="34">
+        <v>6</v>
+      </c>
+      <c r="G72" s="34">
+        <v>4</v>
+      </c>
+      <c r="H72" s="34">
+        <v>0</v>
+      </c>
+      <c r="I72" s="34">
+        <v>1</v>
+      </c>
+      <c r="J72" s="34">
+        <v>40</v>
+      </c>
+      <c r="K72" s="34">
+        <v>50</v>
+      </c>
+      <c r="L72" s="34">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="73" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A73" s="34" t="s">
+        <v>356</v>
+      </c>
+      <c r="B73" s="34">
+        <v>4</v>
+      </c>
+      <c r="C73" s="34">
+        <v>1</v>
+      </c>
+      <c r="D73" s="34">
+        <v>0</v>
+      </c>
+      <c r="E73" s="34">
+        <v>0</v>
+      </c>
+      <c r="F73" s="34">
+        <v>6</v>
+      </c>
+      <c r="G73" s="34">
+        <v>6</v>
+      </c>
+      <c r="H73" s="34">
+        <v>0</v>
+      </c>
+      <c r="I73" s="34">
+        <v>0</v>
+      </c>
+      <c r="J73" s="34">
+        <v>41</v>
+      </c>
+      <c r="K73" s="34">
+        <v>50</v>
+      </c>
+      <c r="L73" s="34">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="74" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A74" s="34" t="s">
+        <v>357</v>
+      </c>
+      <c r="B74" s="34">
+        <v>3</v>
+      </c>
+      <c r="C74" s="34">
+        <v>0</v>
+      </c>
+      <c r="D74" s="34">
+        <v>0</v>
+      </c>
+      <c r="E74" s="34">
+        <v>0</v>
+      </c>
+      <c r="F74" s="34">
+        <v>5</v>
+      </c>
+      <c r="G74" s="34">
+        <v>4</v>
+      </c>
+      <c r="H74" s="34">
+        <v>0</v>
+      </c>
+      <c r="I74" s="34">
+        <v>0</v>
+      </c>
+      <c r="J74" s="34">
+        <v>42</v>
+      </c>
+      <c r="K74" s="34">
+        <v>50</v>
+      </c>
+      <c r="L74" s="34">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="75" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A75" s="34" t="s">
+        <v>358</v>
+      </c>
+      <c r="B75" s="34">
+        <v>6</v>
+      </c>
+      <c r="C75" s="34">
+        <v>1</v>
+      </c>
+      <c r="D75" s="34">
+        <v>1</v>
+      </c>
+      <c r="E75" s="34">
+        <v>0</v>
+      </c>
+      <c r="F75" s="34">
+        <v>6</v>
+      </c>
+      <c r="G75" s="34">
+        <v>6</v>
+      </c>
+      <c r="H75" s="34">
+        <v>0</v>
+      </c>
+      <c r="I75" s="34">
+        <v>0</v>
+      </c>
+      <c r="J75" s="34">
+        <v>32</v>
+      </c>
+      <c r="K75" s="34">
+        <v>44</v>
+      </c>
+      <c r="L75" s="34">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="76" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A76" s="35">
+        <v>74</v>
+      </c>
+      <c r="B76" s="35">
+        <f>SUM(B2:B75)</f>
+        <v>601</v>
+      </c>
+      <c r="C76" s="35">
+        <f t="shared" ref="C76:L76" si="0">SUM(C2:C75)</f>
+        <v>6</v>
+      </c>
+      <c r="D76" s="35">
+        <f t="shared" si="0"/>
+        <v>41</v>
+      </c>
+      <c r="E76" s="35">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F76" s="35">
+        <f t="shared" si="0"/>
+        <v>37</v>
+      </c>
+      <c r="G76" s="35">
+        <f t="shared" si="0"/>
+        <v>270</v>
+      </c>
+      <c r="H76" s="35">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I76" s="35">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="J76" s="35">
+        <f t="shared" si="0"/>
+        <v>2992</v>
+      </c>
+      <c r="K76" s="35">
+        <f t="shared" si="0"/>
+        <v>3665</v>
+      </c>
+      <c r="L76" s="35">
+        <f t="shared" si="0"/>
+        <v>4301</v>
+      </c>
+    </row>
+    <row r="77" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="E77" t="s">
+        <v>12</v>
+      </c>
+      <c r="F77">
+        <f>G76</f>
+        <v>270</v>
+      </c>
+      <c r="J77">
+        <f>B76-C76</f>
+        <v>595</v>
+      </c>
+    </row>
+    <row r="78" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="E78" t="s">
+        <v>13</v>
+      </c>
+      <c r="F78">
+        <f>B76</f>
+        <v>601</v>
+      </c>
+      <c r="J78">
+        <f>D76-E76</f>
+        <v>41</v>
+      </c>
+    </row>
+    <row r="79" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="E79" t="s">
+        <v>14</v>
+      </c>
+      <c r="F79">
+        <v>32</v>
+      </c>
+      <c r="J79">
+        <f>F85</f>
+        <v>3665</v>
+      </c>
+    </row>
+    <row r="80" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="E80" t="s">
+        <v>15</v>
+      </c>
+      <c r="F80">
+        <v>9</v>
+      </c>
+      <c r="J80" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="81" spans="6:10" x14ac:dyDescent="0.25">
+      <c r="F81" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="J81">
+        <f>SUM(J77:J80)</f>
+        <v>4301</v>
+      </c>
+    </row>
+    <row r="82" spans="6:10" x14ac:dyDescent="0.25">
+      <c r="F82">
+        <f>SUM(F77:F81)</f>
+        <v>912</v>
+      </c>
+      <c r="J82" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="83" spans="6:10" x14ac:dyDescent="0.25">
+      <c r="F83">
+        <f>K76-F82</f>
+        <v>2753</v>
+      </c>
+      <c r="J83">
+        <f>J81-L76</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="84" spans="6:10" x14ac:dyDescent="0.25">
+      <c r="F84" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="85" spans="6:10" x14ac:dyDescent="0.25">
+      <c r="F85">
+        <f>F83+F82</f>
+        <v>3665</v>
+      </c>
+    </row>
+    <row r="86" spans="6:10" x14ac:dyDescent="0.25">
+      <c r="F86">
+        <f>F85-K76</f>
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:K9"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
nmv 23 08 2022
</commit_message>
<xml_diff>
--- a/TS Jatai Ghanam Project/Stas table for TS 2.1 TO 2.6.xlsx
+++ b/TS Jatai Ghanam Project/Stas table for TS 2.1 TO 2.6.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="539" uniqueCount="429">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="603" uniqueCount="439">
   <si>
     <t>Panchaati Ref</t>
   </si>
@@ -2424,12 +2424,141 @@
       <t xml:space="preserve">   </t>
     </r>
   </si>
+  <si>
+    <t xml:space="preserve">C¥r | Zûx | D¦ª¥R |   </t>
+  </si>
+  <si>
+    <r>
+      <t>GZy = (B+CZy) |</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">  </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="BRH Malayalam"/>
+        <family val="4"/>
+      </rPr>
+      <t>D¥eZy = (De+CZy)  ¥öeZy = (öe+CZy) |</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">     </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>DexjpJ = Dexjp CZõ¡e - BjpJ |</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">  </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="BRH Malayalam"/>
+        <family val="4"/>
+      </rPr>
+      <t xml:space="preserve">gxt¡hõxI=gxt¡hõxiyZy gxt¡-hõxI </t>
+    </r>
+  </si>
+  <si>
+    <t>¥Z = (¥Z CZy) | ¥Zû = (¥Zû CZy) | P±¡rz = (P±¡rz CZy) | py¥rêx = py¥rêx CZy |</t>
+  </si>
+  <si>
+    <t>Acyrp¥Y = Acyrp¥Y CZõcy - sp¥d | CöÉx²z = CöÉx²z CZzöÉ-A²z |</t>
+  </si>
+  <si>
+    <t xml:space="preserve">இஷே | த்3வா | ஊர்‍ஜே |   </t>
+  </si>
+  <si>
+    <t>ஏதி = (ஆ+இதி)  | உபேதி = (உப+இதி) | ப்ரேதி = (ப்ர+இதி) |</t>
+  </si>
+  <si>
+    <t>தே = (தே இதி)  | த்வே = (த்வே இதி)  | சக்ஷுஷீ = (சக்ஷுஷீ இதி) | விஷ்ணோ = (விஷ்ணோ இதி)  |</t>
+  </si>
+  <si>
+    <t xml:space="preserve">அதி4ஷவணே = அதி4ஷவணே இத்யதி4 - ஸவனே | இந்த்3ராக்3னீ = இந்த்3ராக்3னீ இதீந்த்3ர - அக்3னீ  </t>
+  </si>
+  <si>
+    <r>
+      <t>உபாயவ</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Latha"/>
+        <family val="2"/>
+      </rPr>
+      <t>:</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Latha"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> =  உபாயவ இத்யுப - ஆயவ</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Latha"/>
+        <family val="2"/>
+      </rPr>
+      <t>:</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Latha"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> | பா3ஹுப்4யாம் = பா3ஹுப்4யாமிதி பா3ஹு -  ப்4யாம்  |  </t>
+    </r>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="14" x14ac:knownFonts="1">
+  <fonts count="21" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2527,6 +2656,55 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="16"/>
+      <color rgb="FF000000"/>
+      <name val="BRH Malayalam"/>
+      <family val="4"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="BRH Malayalam"/>
+      <family val="4"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="BRH Malayalam"/>
+      <family val="4"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Latha"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Latha"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Latha"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="6">
     <fill>
@@ -2560,7 +2738,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -2607,11 +2785,20 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
@@ -2710,6 +2897,37 @@
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -18918,17 +19136,17 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:K9"/>
+  <dimension ref="B1:K30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:K8"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="7" customWidth="1"/>
     <col min="3" max="3" width="4.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="21.7109375" customWidth="1"/>
+    <col min="4" max="4" width="23.140625" customWidth="1"/>
     <col min="5" max="5" width="6.7109375" customWidth="1"/>
     <col min="6" max="6" width="7.42578125" customWidth="1"/>
     <col min="7" max="7" width="7" customWidth="1"/>
@@ -19027,7 +19245,7 @@
         <v>14623</v>
       </c>
     </row>
-    <row r="4" spans="2:11" ht="28.5" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:11" ht="42.75" x14ac:dyDescent="0.25">
       <c r="B4" s="31" t="s">
         <v>421</v>
       </c>
@@ -19060,7 +19278,7 @@
         <v>1475</v>
       </c>
     </row>
-    <row r="5" spans="2:11" ht="42.75" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:11" ht="57" x14ac:dyDescent="0.25">
       <c r="B5" s="31" t="s">
         <v>423</v>
       </c>
@@ -19093,7 +19311,7 @@
         <v>3015</v>
       </c>
     </row>
-    <row r="6" spans="2:11" ht="28.5" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:11" ht="55.5" x14ac:dyDescent="0.25">
       <c r="B6" s="31" t="s">
         <v>424</v>
       </c>
@@ -19197,7 +19415,523 @@
     <row r="9" spans="2:11" x14ac:dyDescent="0.25">
       <c r="E9" s="3"/>
     </row>
+    <row r="12" spans="2:11" ht="51.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B12" s="23"/>
+      <c r="C12" s="23"/>
+      <c r="D12" s="23"/>
+      <c r="E12" s="24" t="s">
+        <v>90</v>
+      </c>
+      <c r="F12" s="24" t="s">
+        <v>91</v>
+      </c>
+      <c r="G12" s="24" t="s">
+        <v>92</v>
+      </c>
+      <c r="H12" s="24" t="s">
+        <v>93</v>
+      </c>
+      <c r="I12" s="24" t="s">
+        <v>94</v>
+      </c>
+      <c r="J12" s="24" t="s">
+        <v>95</v>
+      </c>
+      <c r="K12" s="24" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="13" spans="2:11" ht="114.75" x14ac:dyDescent="0.25">
+      <c r="B13" s="25" t="s">
+        <v>18</v>
+      </c>
+      <c r="C13" s="43"/>
+      <c r="D13" s="44" t="s">
+        <v>19</v>
+      </c>
+      <c r="E13" s="28" t="s">
+        <v>20</v>
+      </c>
+      <c r="F13" s="28" t="s">
+        <v>97</v>
+      </c>
+      <c r="G13" s="29" t="s">
+        <v>20</v>
+      </c>
+      <c r="H13" s="29" t="s">
+        <v>20</v>
+      </c>
+      <c r="I13" s="29" t="s">
+        <v>20</v>
+      </c>
+      <c r="J13" s="28" t="s">
+        <v>20</v>
+      </c>
+      <c r="K13" s="29" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="14" spans="2:11" ht="28.5" x14ac:dyDescent="0.25">
+      <c r="B14" s="31" t="s">
+        <v>419</v>
+      </c>
+      <c r="C14" s="30" t="s">
+        <v>21</v>
+      </c>
+      <c r="D14" s="40" t="s">
+        <v>429</v>
+      </c>
+      <c r="E14" s="32">
+        <v>2493</v>
+      </c>
+      <c r="F14" s="32">
+        <v>2524</v>
+      </c>
+      <c r="G14" s="32">
+        <v>2320</v>
+      </c>
+      <c r="H14" s="32">
+        <v>1924</v>
+      </c>
+      <c r="I14" s="32">
+        <v>2753</v>
+      </c>
+      <c r="J14" s="32">
+        <v>2609</v>
+      </c>
+      <c r="K14" s="32">
+        <f>SUM(E14:J14)</f>
+        <v>14623</v>
+      </c>
+    </row>
+    <row r="15" spans="2:11" ht="49.5" x14ac:dyDescent="0.35">
+      <c r="B15" s="31" t="s">
+        <v>421</v>
+      </c>
+      <c r="C15" s="30" t="s">
+        <v>6</v>
+      </c>
+      <c r="D15" s="41" t="s">
+        <v>430</v>
+      </c>
+      <c r="E15" s="32">
+        <v>279</v>
+      </c>
+      <c r="F15" s="32">
+        <v>283</v>
+      </c>
+      <c r="G15" s="32">
+        <v>216</v>
+      </c>
+      <c r="H15" s="32">
+        <v>178</v>
+      </c>
+      <c r="I15" s="32">
+        <v>270</v>
+      </c>
+      <c r="J15" s="32">
+        <v>249</v>
+      </c>
+      <c r="K15" s="32">
+        <f t="shared" ref="K15:K18" si="2">SUM(E15:J15)</f>
+        <v>1475</v>
+      </c>
+    </row>
+    <row r="16" spans="2:11" ht="66" x14ac:dyDescent="0.35">
+      <c r="B16" s="31" t="s">
+        <v>423</v>
+      </c>
+      <c r="C16" s="30" t="s">
+        <v>1</v>
+      </c>
+      <c r="D16" s="42" t="s">
+        <v>431</v>
+      </c>
+      <c r="E16" s="32">
+        <v>498</v>
+      </c>
+      <c r="F16" s="32">
+        <v>681</v>
+      </c>
+      <c r="G16" s="32">
+        <v>402</v>
+      </c>
+      <c r="H16" s="32">
+        <v>295</v>
+      </c>
+      <c r="I16" s="32">
+        <v>601</v>
+      </c>
+      <c r="J16" s="32">
+        <v>538</v>
+      </c>
+      <c r="K16" s="32">
+        <f t="shared" si="2"/>
+        <v>3015</v>
+      </c>
+    </row>
+    <row r="17" spans="2:11" ht="103.5" x14ac:dyDescent="0.25">
+      <c r="B17" s="31" t="s">
+        <v>424</v>
+      </c>
+      <c r="C17" s="30" t="s">
+        <v>3</v>
+      </c>
+      <c r="D17" s="45" t="s">
+        <v>432</v>
+      </c>
+      <c r="E17" s="32">
+        <v>5</v>
+      </c>
+      <c r="F17" s="32">
+        <v>22</v>
+      </c>
+      <c r="G17" s="32">
+        <v>12</v>
+      </c>
+      <c r="H17" s="32">
+        <v>7</v>
+      </c>
+      <c r="I17" s="32">
+        <v>32</v>
+      </c>
+      <c r="J17" s="32">
+        <v>23</v>
+      </c>
+      <c r="K17" s="32">
+        <f t="shared" si="2"/>
+        <v>101</v>
+      </c>
+    </row>
+    <row r="18" spans="2:11" ht="103.5" x14ac:dyDescent="0.25">
+      <c r="B18" s="31" t="s">
+        <v>426</v>
+      </c>
+      <c r="C18" s="30" t="s">
+        <v>22</v>
+      </c>
+      <c r="D18" s="46" t="s">
+        <v>433</v>
+      </c>
+      <c r="E18" s="32">
+        <v>3</v>
+      </c>
+      <c r="F18" s="32">
+        <v>16</v>
+      </c>
+      <c r="G18" s="32">
+        <v>15</v>
+      </c>
+      <c r="H18" s="32">
+        <v>2</v>
+      </c>
+      <c r="I18" s="32">
+        <v>9</v>
+      </c>
+      <c r="J18" s="32">
+        <v>14</v>
+      </c>
+      <c r="K18" s="32">
+        <f t="shared" si="2"/>
+        <v>59</v>
+      </c>
+    </row>
+    <row r="19" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B19" s="34"/>
+      <c r="C19" s="34"/>
+      <c r="D19" s="35" t="s">
+        <v>23</v>
+      </c>
+      <c r="E19" s="36">
+        <f>SUM(E14:E18)</f>
+        <v>3278</v>
+      </c>
+      <c r="F19" s="36">
+        <f t="shared" ref="F19:K19" si="3">SUM(F14:F18)</f>
+        <v>3526</v>
+      </c>
+      <c r="G19" s="36">
+        <f t="shared" si="3"/>
+        <v>2965</v>
+      </c>
+      <c r="H19" s="36">
+        <f t="shared" si="3"/>
+        <v>2406</v>
+      </c>
+      <c r="I19" s="36">
+        <f t="shared" si="3"/>
+        <v>3665</v>
+      </c>
+      <c r="J19" s="36">
+        <f t="shared" si="3"/>
+        <v>3433</v>
+      </c>
+      <c r="K19" s="36">
+        <f t="shared" si="3"/>
+        <v>19273</v>
+      </c>
+    </row>
+    <row r="20" spans="2:11" ht="22.5" x14ac:dyDescent="0.45">
+      <c r="D20" s="39"/>
+    </row>
+    <row r="23" spans="2:11" ht="51.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B23" s="23"/>
+      <c r="C23" s="23"/>
+      <c r="D23" s="23"/>
+      <c r="E23" s="24" t="s">
+        <v>90</v>
+      </c>
+      <c r="F23" s="24" t="s">
+        <v>91</v>
+      </c>
+      <c r="G23" s="24" t="s">
+        <v>92</v>
+      </c>
+      <c r="H23" s="24" t="s">
+        <v>93</v>
+      </c>
+      <c r="I23" s="24" t="s">
+        <v>94</v>
+      </c>
+      <c r="J23" s="24" t="s">
+        <v>95</v>
+      </c>
+      <c r="K23" s="24" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="24" spans="2:11" ht="114.75" x14ac:dyDescent="0.25">
+      <c r="B24" s="25" t="s">
+        <v>18</v>
+      </c>
+      <c r="C24" s="26"/>
+      <c r="D24" s="27" t="s">
+        <v>19</v>
+      </c>
+      <c r="E24" s="28" t="s">
+        <v>20</v>
+      </c>
+      <c r="F24" s="28" t="s">
+        <v>97</v>
+      </c>
+      <c r="G24" s="29" t="s">
+        <v>20</v>
+      </c>
+      <c r="H24" s="29" t="s">
+        <v>20</v>
+      </c>
+      <c r="I24" s="29" t="s">
+        <v>20</v>
+      </c>
+      <c r="J24" s="28" t="s">
+        <v>20</v>
+      </c>
+      <c r="K24" s="29" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="25" spans="2:11" ht="39" x14ac:dyDescent="0.5">
+      <c r="B25" s="31" t="s">
+        <v>419</v>
+      </c>
+      <c r="C25" s="30" t="s">
+        <v>21</v>
+      </c>
+      <c r="D25" s="48" t="s">
+        <v>434</v>
+      </c>
+      <c r="E25" s="32">
+        <v>2493</v>
+      </c>
+      <c r="F25" s="32">
+        <v>2524</v>
+      </c>
+      <c r="G25" s="32">
+        <v>2320</v>
+      </c>
+      <c r="H25" s="32">
+        <v>1924</v>
+      </c>
+      <c r="I25" s="32">
+        <v>2753</v>
+      </c>
+      <c r="J25" s="32">
+        <v>2609</v>
+      </c>
+      <c r="K25" s="32">
+        <f>SUM(E25:J25)</f>
+        <v>14623</v>
+      </c>
+    </row>
+    <row r="26" spans="2:11" ht="58.5" x14ac:dyDescent="0.5">
+      <c r="B26" s="31" t="s">
+        <v>421</v>
+      </c>
+      <c r="C26" s="30" t="s">
+        <v>6</v>
+      </c>
+      <c r="D26" s="48" t="s">
+        <v>435</v>
+      </c>
+      <c r="E26" s="32">
+        <v>279</v>
+      </c>
+      <c r="F26" s="32">
+        <v>283</v>
+      </c>
+      <c r="G26" s="32">
+        <v>216</v>
+      </c>
+      <c r="H26" s="32">
+        <v>178</v>
+      </c>
+      <c r="I26" s="32">
+        <v>270</v>
+      </c>
+      <c r="J26" s="32">
+        <v>249</v>
+      </c>
+      <c r="K26" s="32">
+        <f t="shared" ref="K26:K29" si="4">SUM(E26:J26)</f>
+        <v>1475</v>
+      </c>
+    </row>
+    <row r="27" spans="2:11" ht="117" x14ac:dyDescent="0.5">
+      <c r="B27" s="31" t="s">
+        <v>423</v>
+      </c>
+      <c r="C27" s="30" t="s">
+        <v>1</v>
+      </c>
+      <c r="D27" s="47" t="s">
+        <v>438</v>
+      </c>
+      <c r="E27" s="32">
+        <v>498</v>
+      </c>
+      <c r="F27" s="32">
+        <v>681</v>
+      </c>
+      <c r="G27" s="32">
+        <v>402</v>
+      </c>
+      <c r="H27" s="32">
+        <v>295</v>
+      </c>
+      <c r="I27" s="32">
+        <v>601</v>
+      </c>
+      <c r="J27" s="32">
+        <v>538</v>
+      </c>
+      <c r="K27" s="32">
+        <f t="shared" si="4"/>
+        <v>3015</v>
+      </c>
+    </row>
+    <row r="28" spans="2:11" ht="117" x14ac:dyDescent="0.5">
+      <c r="B28" s="31" t="s">
+        <v>424</v>
+      </c>
+      <c r="C28" s="30" t="s">
+        <v>3</v>
+      </c>
+      <c r="D28" s="49" t="s">
+        <v>436</v>
+      </c>
+      <c r="E28" s="32">
+        <v>5</v>
+      </c>
+      <c r="F28" s="32">
+        <v>22</v>
+      </c>
+      <c r="G28" s="32">
+        <v>12</v>
+      </c>
+      <c r="H28" s="32">
+        <v>7</v>
+      </c>
+      <c r="I28" s="32">
+        <v>32</v>
+      </c>
+      <c r="J28" s="32">
+        <v>23</v>
+      </c>
+      <c r="K28" s="32">
+        <f t="shared" si="4"/>
+        <v>101</v>
+      </c>
+    </row>
+    <row r="29" spans="2:11" ht="117" x14ac:dyDescent="0.5">
+      <c r="B29" s="31" t="s">
+        <v>426</v>
+      </c>
+      <c r="C29" s="30" t="s">
+        <v>22</v>
+      </c>
+      <c r="D29" s="48" t="s">
+        <v>437</v>
+      </c>
+      <c r="E29" s="32">
+        <v>3</v>
+      </c>
+      <c r="F29" s="32">
+        <v>16</v>
+      </c>
+      <c r="G29" s="32">
+        <v>15</v>
+      </c>
+      <c r="H29" s="32">
+        <v>2</v>
+      </c>
+      <c r="I29" s="32">
+        <v>9</v>
+      </c>
+      <c r="J29" s="32">
+        <v>14</v>
+      </c>
+      <c r="K29" s="32">
+        <f t="shared" si="4"/>
+        <v>59</v>
+      </c>
+    </row>
+    <row r="30" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B30" s="34"/>
+      <c r="C30" s="34"/>
+      <c r="D30" s="35" t="s">
+        <v>23</v>
+      </c>
+      <c r="E30" s="36">
+        <f>SUM(E25:E29)</f>
+        <v>3278</v>
+      </c>
+      <c r="F30" s="36">
+        <f t="shared" ref="F30:K30" si="5">SUM(F25:F29)</f>
+        <v>3526</v>
+      </c>
+      <c r="G30" s="36">
+        <f t="shared" si="5"/>
+        <v>2965</v>
+      </c>
+      <c r="H30" s="36">
+        <f t="shared" si="5"/>
+        <v>2406</v>
+      </c>
+      <c r="I30" s="36">
+        <f t="shared" si="5"/>
+        <v>3665</v>
+      </c>
+      <c r="J30" s="36">
+        <f t="shared" si="5"/>
+        <v>3433</v>
+      </c>
+      <c r="K30" s="36">
+        <f t="shared" si="5"/>
+        <v>19273</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
nmv 12 09 2022
</commit_message>
<xml_diff>
--- a/TS Jatai Ghanam Project/Stas table for TS 2.1 TO 2.6.xlsx
+++ b/TS Jatai Ghanam Project/Stas table for TS 2.1 TO 2.6.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7095" activeTab="6"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7095" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="TS 2.1" sheetId="8" r:id="rId1"/>
@@ -2706,7 +2706,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2734,6 +2734,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2798,7 +2804,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="50">
+  <cellXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
@@ -2928,6 +2934,9 @@
     </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -5957,9 +5966,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L83"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A68" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" sqref="A1:L73"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A62" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I70" sqref="I70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8623,8 +8632,8 @@
       <c r="H70" s="9">
         <v>0</v>
       </c>
-      <c r="I70" s="9">
-        <v>0</v>
+      <c r="I70" s="50">
+        <v>1</v>
       </c>
       <c r="J70" s="9">
         <v>39</v>
@@ -8746,7 +8755,7 @@
       </c>
       <c r="I73" s="12">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="J73" s="12">
         <f t="shared" si="0"/>
@@ -19138,7 +19147,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:K30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+    <sheetView topLeftCell="A28" workbookViewId="0">
       <selection activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
@@ -19245,7 +19254,7 @@
         <v>14623</v>
       </c>
     </row>
-    <row r="4" spans="2:11" ht="42.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:11" ht="28.5" x14ac:dyDescent="0.25">
       <c r="B4" s="31" t="s">
         <v>421</v>
       </c>
@@ -19278,7 +19287,7 @@
         <v>1475</v>
       </c>
     </row>
-    <row r="5" spans="2:11" ht="57" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:11" ht="42.75" x14ac:dyDescent="0.25">
       <c r="B5" s="31" t="s">
         <v>423</v>
       </c>
@@ -19311,7 +19320,7 @@
         <v>3015</v>
       </c>
     </row>
-    <row r="6" spans="2:11" ht="55.5" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:11" ht="41.25" x14ac:dyDescent="0.25">
       <c r="B6" s="31" t="s">
         <v>424</v>
       </c>

</xml_diff>